<commit_message>
fix typo in financials + add missing kicad files
</commit_message>
<xml_diff>
--- a/Hardware/Estimated Financials.xlsx
+++ b/Hardware/Estimated Financials.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Josh Johnson\Dropbox\ENGN4221\VeinCam2019\Hardware\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jonno\Dropbox\ENGN4221\VeinCam2019\Hardware\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{B57FAA91-2B19-4B2F-90A0-F32CFC5E3CBE}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2BAC434B-72CC-4D03-98AE-256DC5DE8280}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="28110" windowHeight="16440"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13276" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="RPi 3A+ Total BOM" sheetId="4" r:id="rId1"/>
@@ -18,12 +18,20 @@
     <sheet name="VeinCamHat BOM" sheetId="1" r:id="rId3"/>
     <sheet name="VeinCamHatZero BOM" sheetId="2" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="205" uniqueCount="143">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="205" uniqueCount="144">
   <si>
     <t>Qty</t>
   </si>
@@ -452,12 +460,15 @@
   </si>
   <si>
     <t>https://core-electronics.com.au/raspberry-pi-3-model-a-plus.html</t>
+  </si>
+  <si>
+    <t>See VeinCamHat Sheet</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="44" formatCode="_-&quot;$&quot;* #,##0.00_-;\-&quot;$&quot;* #,##0.00_-;_-&quot;$&quot;* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
@@ -955,20 +966,20 @@
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="44"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="2" applyFont="1"/>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="44"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="2" applyFont="1"/>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="45">
@@ -1327,32 +1338,32 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E25" sqref="E25"/>
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="2" max="2" width="22.140625" customWidth="1"/>
-    <col min="3" max="3" width="14.42578125" customWidth="1"/>
+    <col min="2" max="2" width="22.1328125" customWidth="1"/>
+    <col min="3" max="3" width="14.3984375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A1" s="6" t="s">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A1" s="9" t="s">
         <v>115</v>
       </c>
-      <c r="B1" s="6"/>
-      <c r="C1" s="6"/>
-    </row>
-    <row r="2" spans="1:11" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="6" t="s">
+      <c r="B1" s="9"/>
+      <c r="C1" s="9"/>
+    </row>
+    <row r="2" spans="1:11" ht="30.75" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A2" s="9" t="s">
         <v>100</v>
       </c>
-      <c r="B2" s="6"/>
-      <c r="C2" s="11" t="s">
+      <c r="B2" s="9"/>
+      <c r="C2" s="8" t="s">
         <v>103</v>
       </c>
       <c r="D2" s="4"/>
@@ -1360,7 +1371,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
         <v>101</v>
       </c>
@@ -1369,16 +1380,16 @@
         <v>46.048200000000008</v>
       </c>
       <c r="E3" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A4" s="5" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A4" s="10" t="s">
         <v>102</v>
       </c>
-      <c r="B4" s="5"/>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B4" s="10"/>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.45">
       <c r="B5" t="s">
         <v>136</v>
       </c>
@@ -1392,7 +1403,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.45">
       <c r="B6" t="s">
         <v>135</v>
       </c>
@@ -1403,7 +1414,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.45">
       <c r="B7" t="s">
         <v>139</v>
       </c>
@@ -1414,27 +1425,27 @@
         <v>140</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A8" t="s">
         <v>106</v>
       </c>
       <c r="C8" s="1">
         <v>2</v>
       </c>
-      <c r="E8" s="7" t="s">
+      <c r="E8" s="5" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.45">
       <c r="C9" s="1"/>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A10" s="8" t="s">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A10" s="11" t="s">
         <v>116</v>
       </c>
-      <c r="B10" s="8"/>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B10" s="11"/>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.45">
       <c r="B11" t="s">
         <v>118</v>
       </c>
@@ -1443,7 +1454,7 @@
         <v>50.848200000000006</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.45">
       <c r="B12" t="s">
         <v>117</v>
       </c>
@@ -1451,25 +1462,25 @@
         <v>150</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.45">
       <c r="B13" t="s">
         <v>120</v>
       </c>
-      <c r="C13" s="10">
+      <c r="C13" s="7">
         <f>C12-C11</f>
         <v>99.151799999999994</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.45">
       <c r="B14" t="s">
         <v>119</v>
       </c>
-      <c r="C14" s="9">
+      <c r="C14" s="6">
         <f>C13/C11</f>
         <v>1.9499569306288125</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.45">
       <c r="B15" t="s">
         <v>121</v>
       </c>
@@ -1477,12 +1488,12 @@
         <v>8.3000000000000007</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A17" s="4" t="s">
         <v>122</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.45">
       <c r="B18" t="s">
         <v>141</v>
       </c>
@@ -1493,7 +1504,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.45">
       <c r="B19" t="s">
         <v>124</v>
       </c>
@@ -1504,18 +1515,18 @@
         <v>127</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.45">
       <c r="B20" t="s">
         <v>125</v>
       </c>
       <c r="C20" s="1">
         <v>9</v>
       </c>
-      <c r="E20" s="7" t="s">
+      <c r="E20" s="5" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.45">
       <c r="B22" t="s">
         <v>130</v>
       </c>
@@ -1524,17 +1535,17 @@
         <v>86.18</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A24" s="4" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.45">
       <c r="B25" t="s">
         <v>132</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.45">
       <c r="B26" s="4" t="s">
         <v>134</v>
       </c>
@@ -1551,42 +1562,42 @@
     <mergeCell ref="A10:B10"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="E8" r:id="rId1"/>
-    <hyperlink ref="E20" r:id="rId2"/>
+    <hyperlink ref="E8" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="E20" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:I28"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C35" sqref="C35"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="9.85546875" customWidth="1"/>
+    <col min="1" max="1" width="9.86328125" customWidth="1"/>
     <col min="2" max="2" width="22" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="5.42578125" customWidth="1"/>
+    <col min="3" max="3" width="14.73046875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="5.3984375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A1" s="6" t="s">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A1" s="9" t="s">
         <v>115</v>
       </c>
-      <c r="B1" s="6"/>
-      <c r="C1" s="6"/>
-    </row>
-    <row r="2" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A2" s="6" t="s">
+      <c r="B1" s="9"/>
+      <c r="C1" s="9"/>
+    </row>
+    <row r="2" spans="1:9" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="A2" s="9" t="s">
         <v>100</v>
       </c>
-      <c r="B2" s="6"/>
-      <c r="C2" s="11" t="s">
+      <c r="B2" s="9"/>
+      <c r="C2" s="8" t="s">
         <v>103</v>
       </c>
       <c r="D2" s="4"/>
@@ -1594,7 +1605,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
         <v>101</v>
       </c>
@@ -1606,13 +1617,13 @@
         <v>108</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A4" s="5" t="s">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A4" s="10" t="s">
         <v>102</v>
       </c>
-      <c r="B4" s="5"/>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B4" s="10"/>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.45">
       <c r="B5" t="s">
         <v>104</v>
       </c>
@@ -1623,7 +1634,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.45">
       <c r="B6" t="s">
         <v>110</v>
       </c>
@@ -1634,7 +1645,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.45">
       <c r="B7" t="s">
         <v>105</v>
       </c>
@@ -1645,30 +1656,30 @@
         <v>112</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A8" t="s">
         <v>106</v>
       </c>
       <c r="C8" s="1">
         <v>2</v>
       </c>
-      <c r="E8" s="7" t="s">
+      <c r="E8" s="5" t="s">
         <v>113</v>
       </c>
       <c r="I8" s="4" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.45">
       <c r="C9" s="1"/>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A10" s="8" t="s">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A10" s="11" t="s">
         <v>116</v>
       </c>
-      <c r="B10" s="8"/>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B10" s="11"/>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.45">
       <c r="B11" t="s">
         <v>118</v>
       </c>
@@ -1677,7 +1688,7 @@
         <v>11.795999999999999</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.45">
       <c r="B12" t="s">
         <v>117</v>
       </c>
@@ -1685,25 +1696,25 @@
         <v>34.99</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.45">
       <c r="B13" t="s">
         <v>120</v>
       </c>
-      <c r="C13" s="10">
+      <c r="C13" s="7">
         <f>C12-C11</f>
         <v>23.194000000000003</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.45">
       <c r="B14" t="s">
         <v>119</v>
       </c>
-      <c r="C14" s="9">
+      <c r="C14" s="6">
         <f>C13/C11</f>
         <v>1.9662597490674809</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.45">
       <c r="B15" t="s">
         <v>121</v>
       </c>
@@ -1711,12 +1722,12 @@
         <v>8.3000000000000007</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A17" s="4" t="s">
         <v>122</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.45">
       <c r="B18" t="s">
         <v>123</v>
       </c>
@@ -1727,7 +1738,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.45">
       <c r="B19" t="s">
         <v>124</v>
       </c>
@@ -1738,18 +1749,18 @@
         <v>127</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.45">
       <c r="B20" t="s">
         <v>125</v>
       </c>
       <c r="C20" s="1">
         <v>9</v>
       </c>
-      <c r="E20" s="7" t="s">
+      <c r="E20" s="5" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.45">
       <c r="B21" t="s">
         <v>126</v>
       </c>
@@ -1760,7 +1771,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.45">
       <c r="B23" t="s">
         <v>130</v>
       </c>
@@ -1769,17 +1780,17 @@
         <v>83.240000000000009</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A25" s="4" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.45">
       <c r="B26" t="s">
         <v>132</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.45">
       <c r="B27" s="4" t="s">
         <v>134</v>
       </c>
@@ -1788,7 +1799,7 @@
         <v>126.53</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.45">
       <c r="C28" s="2"/>
     </row>
   </sheetData>
@@ -1799,8 +1810,8 @@
     <mergeCell ref="A10:B10"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="E8" r:id="rId1"/>
-    <hyperlink ref="E20" r:id="rId2"/>
+    <hyperlink ref="E8" r:id="rId1" xr:uid="{00000000-0004-0000-0100-000000000000}"/>
+    <hyperlink ref="E20" r:id="rId2" xr:uid="{00000000-0004-0000-0100-000001000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId3"/>
@@ -1808,25 +1819,25 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:I33"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A32" sqref="A32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="2" max="2" width="29.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="29.73046875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="22" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="27.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.73046875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="27.265625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="14" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="19.5703125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="19.59765625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.1328125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1852,7 +1863,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A2">
         <v>1</v>
       </c>
@@ -1880,7 +1891,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A3">
         <v>4</v>
       </c>
@@ -1891,14 +1902,14 @@
         <v>5</v>
       </c>
       <c r="D3">
-        <f t="shared" ref="D3:D30" si="0">1000*A3</f>
+        <f t="shared" ref="D3:D29" si="0">1000*A3</f>
         <v>4000</v>
       </c>
       <c r="E3" s="1">
         <v>0.05</v>
       </c>
       <c r="F3" s="1">
-        <f t="shared" ref="F3:F30" si="1">E3*A3</f>
+        <f t="shared" ref="F3:F26" si="1">E3*A3</f>
         <v>0.2</v>
       </c>
       <c r="G3" s="3"/>
@@ -1906,7 +1917,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A4">
         <v>2</v>
       </c>
@@ -1932,7 +1943,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A5">
         <v>1</v>
       </c>
@@ -1958,7 +1969,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A6">
         <v>1</v>
       </c>
@@ -1984,7 +1995,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A7">
         <v>6</v>
       </c>
@@ -2012,7 +2023,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A8">
         <v>3</v>
       </c>
@@ -2038,7 +2049,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A9">
         <v>3</v>
       </c>
@@ -2064,7 +2075,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A10">
         <v>1</v>
       </c>
@@ -2090,7 +2101,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A11">
         <v>1</v>
       </c>
@@ -2118,7 +2129,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A12">
         <v>1</v>
       </c>
@@ -2144,7 +2155,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A13">
         <v>1</v>
       </c>
@@ -2170,7 +2181,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A14">
         <v>1</v>
       </c>
@@ -2196,7 +2207,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A15">
         <v>4</v>
       </c>
@@ -2222,7 +2233,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A16">
         <v>4</v>
       </c>
@@ -2248,7 +2259,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A17">
         <v>7</v>
       </c>
@@ -2274,7 +2285,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A18">
         <v>1</v>
       </c>
@@ -2300,7 +2311,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A19">
         <v>1</v>
       </c>
@@ -2326,7 +2337,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A20">
         <v>1</v>
       </c>
@@ -2352,7 +2363,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A21">
         <v>2</v>
       </c>
@@ -2378,7 +2389,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A22">
         <v>1</v>
       </c>
@@ -2404,7 +2415,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A23">
         <v>1</v>
       </c>
@@ -2430,7 +2441,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A24">
         <v>1</v>
       </c>
@@ -2456,7 +2467,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A25">
         <v>1</v>
       </c>
@@ -2482,7 +2493,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A26">
         <v>1</v>
       </c>
@@ -2508,14 +2519,14 @@
         <v>89</v>
       </c>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.45">
       <c r="E27" s="1" t="s">
         <v>99</v>
       </c>
       <c r="F27" s="1"/>
       <c r="G27" s="3"/>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A28">
         <v>1</v>
       </c>
@@ -2537,7 +2548,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A29">
         <v>1</v>
       </c>
@@ -2559,7 +2570,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A30">
         <v>1</v>
       </c>
@@ -2580,10 +2591,10 @@
         <v>91</v>
       </c>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.45">
       <c r="G31" s="3"/>
     </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:9" x14ac:dyDescent="0.45">
       <c r="E32" t="s">
         <v>58</v>
       </c>
@@ -2592,7 +2603,7 @@
         <v>41.862000000000002</v>
       </c>
     </row>
-    <row r="33" spans="5:6" x14ac:dyDescent="0.25">
+    <row r="33" spans="5:6" x14ac:dyDescent="0.45">
       <c r="E33" t="s">
         <v>59</v>
       </c>
@@ -2607,24 +2618,24 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:I16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="2" max="2" width="29.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="27.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="29.73046875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.3984375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.73046875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="27.265625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="14" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="17.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="17.3984375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2650,7 +2661,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A2">
         <v>5</v>
       </c>
@@ -2668,7 +2679,7 @@
         <v>0.86</v>
       </c>
       <c r="F2" s="1">
-        <f t="shared" ref="F2:F13" si="1">E2*A2</f>
+        <f t="shared" ref="F2:F8" si="1">E2*A2</f>
         <v>4.3</v>
       </c>
       <c r="G2" s="3" t="s">
@@ -2678,7 +2689,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A3">
         <v>1</v>
       </c>
@@ -2704,7 +2715,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A4">
         <v>1</v>
       </c>
@@ -2730,7 +2741,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A5">
         <v>1</v>
       </c>
@@ -2756,7 +2767,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A6">
         <v>2</v>
       </c>
@@ -2782,7 +2793,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A7">
         <v>2</v>
       </c>
@@ -2808,7 +2819,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A8">
         <v>2</v>
       </c>
@@ -2834,7 +2845,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A9">
         <v>2</v>
       </c>
@@ -2860,14 +2871,14 @@
         <v>98</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.45">
       <c r="E10" s="1" t="s">
         <v>99</v>
       </c>
       <c r="F10" s="1"/>
       <c r="G10" s="3"/>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A11">
         <v>1</v>
       </c>
@@ -2889,7 +2900,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A12">
         <v>1</v>
       </c>
@@ -2911,7 +2922,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A13">
         <v>1</v>
       </c>
@@ -2932,10 +2943,10 @@
         <v>91</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.45">
       <c r="G14" s="3"/>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.45">
       <c r="E15" t="s">
         <v>58</v>
       </c>
@@ -2944,7 +2955,7 @@
         <v>5.3599999999999985</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.45">
       <c r="E16" t="s">
         <v>59</v>
       </c>

</xml_diff>

<commit_message>
Changed plans for VeinCam Plus, both boards laid out
</commit_message>
<xml_diff>
--- a/Hardware/Estimated Financials.xlsx
+++ b/Hardware/Estimated Financials.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Josh Johnson\Dropbox\ENGN4221\VeinCam2019\Hardware\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{44F7D212-AC36-49E3-B13A-596B05D78E16}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8AFD329F-6269-4957-BA19-AE974998079C}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="28110" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="RPi 3A+ Total BOM" sheetId="4" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="205" uniqueCount="144">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="93">
   <si>
     <t>Qty</t>
   </si>
@@ -42,30 +42,6 @@
     <t>Value</t>
   </si>
   <si>
-    <t>BT1</t>
-  </si>
-  <si>
-    <t>3v7 LIPO</t>
-  </si>
-  <si>
-    <t>10u</t>
-  </si>
-  <si>
-    <t>100n</t>
-  </si>
-  <si>
-    <t>C6</t>
-  </si>
-  <si>
-    <t>2u2</t>
-  </si>
-  <si>
-    <t>C7</t>
-  </si>
-  <si>
-    <t>100u</t>
-  </si>
-  <si>
     <t>SFH7252</t>
   </si>
   <si>
@@ -75,33 +51,15 @@
     <t>RED LED</t>
   </si>
   <si>
-    <t>J1</t>
-  </si>
-  <si>
-    <t>USB_B_Micro</t>
-  </si>
-  <si>
     <t>J2</t>
   </si>
   <si>
-    <t>L1</t>
-  </si>
-  <si>
-    <t>6u8</t>
-  </si>
-  <si>
     <t>Q1</t>
   </si>
   <si>
     <t>BSD235N</t>
   </si>
   <si>
-    <t>Q2</t>
-  </si>
-  <si>
-    <t>MMUN2133L</t>
-  </si>
-  <si>
     <t>3R3</t>
   </si>
   <si>
@@ -111,66 +69,6 @@
     <t>1k</t>
   </si>
   <si>
-    <t>R17</t>
-  </si>
-  <si>
-    <t>1M87</t>
-  </si>
-  <si>
-    <t>R18</t>
-  </si>
-  <si>
-    <t>340k</t>
-  </si>
-  <si>
-    <t>R19</t>
-  </si>
-  <si>
-    <t>270k</t>
-  </si>
-  <si>
-    <t>100k</t>
-  </si>
-  <si>
-    <t>SW1</t>
-  </si>
-  <si>
-    <t>SW_SPST</t>
-  </si>
-  <si>
-    <t>TH1</t>
-  </si>
-  <si>
-    <t>10k NTC</t>
-  </si>
-  <si>
-    <t>U1</t>
-  </si>
-  <si>
-    <t>MCP3021</t>
-  </si>
-  <si>
-    <t>U2</t>
-  </si>
-  <si>
-    <t>TPS61092</t>
-  </si>
-  <si>
-    <t>U3</t>
-  </si>
-  <si>
-    <t>MCP73871</t>
-  </si>
-  <si>
-    <t>C1, C3, C4, C8</t>
-  </si>
-  <si>
-    <t>C2, C5</t>
-  </si>
-  <si>
-    <t>D1, D2, D3, D4, D5, D6</t>
-  </si>
-  <si>
     <t>D7, D9, D11</t>
   </si>
   <si>
@@ -180,15 +78,6 @@
     <t>R3, R4, R5, R6</t>
   </si>
   <si>
-    <t>R8, R9, R10, R14</t>
-  </si>
-  <si>
-    <t>R11, R12, R13, R15, R16, R21, R23</t>
-  </si>
-  <si>
-    <t>R20, R22</t>
-  </si>
-  <si>
     <t>Quantity Per 1000</t>
   </si>
   <si>
@@ -213,60 +102,30 @@
     <t>Total Per Board (inc):</t>
   </si>
   <si>
-    <t>https://au.element14.com/mikroelektronika/mikroe-1120/lithium-polymer-battery-3-7v-2ah/dp/2786900</t>
-  </si>
-  <si>
     <t>Notes</t>
   </si>
   <si>
-    <t>Price @ Q = 1</t>
-  </si>
-  <si>
     <t>https://au.rs-online.com/web/p/ir-leds/1685175/</t>
   </si>
   <si>
     <t>5 month lead time</t>
   </si>
   <si>
-    <t>https://www.digikey.com.au/product-detail/en/murata-electronics-north-america/GRM188R61A106KE69D/490-10474-2-ND/5027559</t>
-  </si>
-  <si>
-    <t>https://www.digikey.com.au/product-detail/en/kemet/C0603C104K8RACTU/399-1095-1-ND/411370</t>
-  </si>
-  <si>
-    <t>https://www.digikey.com.au/product-detail/en/samsung-electro-mechanics/CL10A225KP8NNNC/1276-1085-1-ND/3889171</t>
-  </si>
-  <si>
-    <t>https://www.digikey.com.au/product-detail/en/avx-corporation/TPSD107M020R0085/478-6066-2-ND/1473072</t>
-  </si>
-  <si>
     <t>https://www.digikey.com.au/products/en/optoelectronics/led-indication-discrete/105?FV=ffe00069&amp;quantity=3000&amp;ColumnSort=1000011&amp;page=1&amp;stock=1&amp;k=0805+green+led&amp;pageSize=25&amp;pkeyword=0805+green+led</t>
   </si>
   <si>
     <t>https://www.digikey.com.au/product-detail/en/lite-on-inc/LTST-C171KRKT/160-1427-2-ND/386801</t>
   </si>
   <si>
-    <t>https://www.digikey.com.au/product-detail/en/amphenol-icc-fci/10118193-0001LF/609-4616-1-ND/2785380</t>
-  </si>
-  <si>
-    <t>20x2 Pin Header Femail</t>
-  </si>
-  <si>
     <t>https://www.digikey.com.au/product-detail/en/sullins-connector-solutions/PPTC202LFBN-RC/S6104-ND/807240</t>
   </si>
   <si>
     <t>&lt;$0.20 ea from China</t>
   </si>
   <si>
-    <t>https://www.digikey.com.au/product-detail/en/on-semiconductor/MMUN2133LT1G/MMUN2133LT1GOSCT-ND/2705149</t>
-  </si>
-  <si>
     <t>https://www.digikey.com.au/product-detail/en/infineon-technologies/BSD235NH6327XTSA1/BSD235NH6327XTSA1CT-ND/3196626</t>
   </si>
   <si>
-    <t>https://www.digikey.com.au/product-detail/en/bourns-inc/SRN6045-6R8Y/SRN6045-6R8YTR-ND/2756118</t>
-  </si>
-  <si>
     <t>https://www.digikey.com.au/product-detail/en/te-connectivity-passive-product/CRGCQ0603J3R3/A130076CT-ND/8577908</t>
   </si>
   <si>
@@ -276,33 +135,6 @@
     <t>https://www.digikey.com.au/product-detail/en/te-connectivity-passive-product/CRGCQ0603J1K0/A130091CT-ND/8577923</t>
   </si>
   <si>
-    <t>https://www.digikey.com.au/product-detail/en/stackpole-electronics-inc/RMCF0603FT1M87/RMCF0603FT1M87CT-ND/7790193</t>
-  </si>
-  <si>
-    <t>https://www.digikey.com.au/product-detail/en/stackpole-electronics-inc/RMCF0603FT340K/RMCF0603FT340KCT-ND/6053163</t>
-  </si>
-  <si>
-    <t>https://www.digikey.com.au/product-detail/en/stackpole-electronics-inc/RMCF0603JT270K/RMCF0603JT270KCT-ND/5050301</t>
-  </si>
-  <si>
-    <t>https://www.digikey.com.au/product-detail/en/stackpole-electronics-inc/RMCF0603JG100K/RMCF0603JG100KCT-ND/4425127</t>
-  </si>
-  <si>
-    <t>https://www.digikey.com.au/products/en/switches/slide-switches/213?k=ss-12d07&amp;k=&amp;pkeyword=ss-12d07&amp;sv=0&amp;sf=0&amp;FV=ffe000d5&amp;quantity=&amp;ColumnSort=0&amp;page=1&amp;stock=1&amp;pageSize=25</t>
-  </si>
-  <si>
-    <t>https://www.digikey.com.au/product-detail/en/murata-electronics-north-america/NCU18XH103F60RB/490-16279-1-ND/7363262</t>
-  </si>
-  <si>
-    <t>https://www.digikey.com.au/product-detail/en/microchip-technology/MCP3021A5T-E-OT/MCP3021A5T-E-OTCT-ND/1979808</t>
-  </si>
-  <si>
-    <t>https://www.digikey.com.au/product-detail/en/texas-instruments/TPS61092RSAR/296-15240-1-ND/566513</t>
-  </si>
-  <si>
-    <t>https://www.digikey.com.au/product-detail/en/microchip-technology/MCP73871-2CCI-ML/MCP73871-2CCI-ML-ND/1680971</t>
-  </si>
-  <si>
     <t>Freight</t>
   </si>
   <si>
@@ -463,6 +295,21 @@
   </si>
   <si>
     <t>See VeinCamHat Sheet</t>
+  </si>
+  <si>
+    <t>20x2 Pin Header Female</t>
+  </si>
+  <si>
+    <t>D1</t>
+  </si>
+  <si>
+    <t>D2</t>
+  </si>
+  <si>
+    <t>D3, D4, D5, D6, D7, D8</t>
+  </si>
+  <si>
+    <t>R7, R8</t>
   </si>
 </sst>
 </file>
@@ -1341,8 +1188,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K26"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1353,87 +1200,87 @@
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" s="9" t="s">
-        <v>115</v>
+        <v>59</v>
       </c>
       <c r="B1" s="9"/>
       <c r="C1" s="9"/>
     </row>
     <row r="2" spans="1:11" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="9" t="s">
-        <v>100</v>
+        <v>44</v>
       </c>
       <c r="B2" s="9"/>
       <c r="C2" s="8" t="s">
-        <v>103</v>
+        <v>47</v>
       </c>
       <c r="D2" s="4"/>
       <c r="E2" t="s">
-        <v>107</v>
+        <v>51</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>101</v>
+        <v>45</v>
       </c>
       <c r="C3" s="2">
-        <f>'VeinCamHat BOM'!F33</f>
-        <v>46.048200000000008</v>
+        <f>'VeinCamHat BOM'!F17</f>
+        <v>9.3940000000000019</v>
       </c>
       <c r="E3" t="s">
-        <v>143</v>
+        <v>87</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" s="10" t="s">
-        <v>102</v>
+        <v>46</v>
       </c>
       <c r="B4" s="10"/>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
-        <v>136</v>
+        <v>80</v>
       </c>
       <c r="C5" s="1">
         <v>1</v>
       </c>
       <c r="E5" t="s">
-        <v>137</v>
+        <v>81</v>
       </c>
       <c r="K5" t="s">
-        <v>138</v>
+        <v>82</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
-        <v>135</v>
+        <v>79</v>
       </c>
       <c r="C6" s="1">
         <v>0.8</v>
       </c>
       <c r="E6" t="s">
-        <v>112</v>
+        <v>56</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
-        <v>139</v>
+        <v>83</v>
       </c>
       <c r="C7" s="1">
         <v>1</v>
       </c>
       <c r="E7" t="s">
-        <v>140</v>
+        <v>84</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>106</v>
+        <v>50</v>
       </c>
       <c r="C8" s="1">
         <v>2</v>
       </c>
       <c r="E8" s="5" t="s">
-        <v>113</v>
+        <v>57</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
@@ -1441,48 +1288,48 @@
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" s="11" t="s">
-        <v>116</v>
+        <v>60</v>
       </c>
       <c r="B10" s="11"/>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
-        <v>118</v>
+        <v>62</v>
       </c>
       <c r="C11" s="1">
         <f>SUM(C3:C8)</f>
-        <v>50.848200000000006</v>
+        <v>14.194000000000003</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
-        <v>117</v>
+        <v>61</v>
       </c>
       <c r="C12" s="1">
-        <v>150</v>
+        <v>39.99</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
-        <v>120</v>
+        <v>64</v>
       </c>
       <c r="C13" s="7">
         <f>C12-C11</f>
-        <v>99.151799999999994</v>
+        <v>25.795999999999999</v>
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
-        <v>119</v>
+        <v>63</v>
       </c>
       <c r="C14" s="6">
         <f>C13/C11</f>
-        <v>1.9499569306288125</v>
+        <v>1.817387628575454</v>
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
-        <v>121</v>
+        <v>65</v>
       </c>
       <c r="C15" s="1">
         <v>8.3000000000000007</v>
@@ -1490,45 +1337,45 @@
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="4" t="s">
-        <v>122</v>
+        <v>66</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B18" t="s">
-        <v>141</v>
+        <v>85</v>
       </c>
       <c r="C18" s="1">
         <v>38.229999999999997</v>
       </c>
       <c r="E18" t="s">
-        <v>142</v>
+        <v>86</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B19" t="s">
-        <v>124</v>
+        <v>68</v>
       </c>
       <c r="C19" s="1">
         <v>38.950000000000003</v>
       </c>
       <c r="E19" t="s">
-        <v>127</v>
+        <v>71</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B20" t="s">
-        <v>125</v>
+        <v>69</v>
       </c>
       <c r="C20" s="1">
         <v>9</v>
       </c>
       <c r="E20" s="5" t="s">
-        <v>129</v>
+        <v>73</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B22" t="s">
-        <v>130</v>
+        <v>74</v>
       </c>
       <c r="C22" s="2">
         <f>SUM(C18:C20)</f>
@@ -1537,21 +1384,21 @@
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" s="4" t="s">
-        <v>133</v>
+        <v>77</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B25" t="s">
-        <v>132</v>
+        <v>76</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B26" s="4" t="s">
-        <v>134</v>
+        <v>78</v>
       </c>
       <c r="C26" s="2">
         <f>C22+C15+C12</f>
-        <v>244.48000000000002</v>
+        <v>134.47</v>
       </c>
     </row>
   </sheetData>
@@ -1587,87 +1434,87 @@
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="9" t="s">
-        <v>115</v>
+        <v>59</v>
       </c>
       <c r="B1" s="9"/>
       <c r="C1" s="9"/>
     </row>
     <row r="2" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" s="9" t="s">
-        <v>100</v>
+        <v>44</v>
       </c>
       <c r="B2" s="9"/>
       <c r="C2" s="8" t="s">
-        <v>103</v>
+        <v>47</v>
       </c>
       <c r="D2" s="4"/>
       <c r="E2" t="s">
-        <v>107</v>
+        <v>51</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>101</v>
+        <v>45</v>
       </c>
       <c r="C3" s="2">
         <f>'VeinCamHatZero BOM'!F16</f>
         <v>5.895999999999999</v>
       </c>
       <c r="E3" t="s">
-        <v>108</v>
+        <v>52</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="10" t="s">
-        <v>102</v>
+        <v>46</v>
       </c>
       <c r="B4" s="10"/>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
-        <v>104</v>
+        <v>48</v>
       </c>
       <c r="C5" s="1">
         <v>3.1</v>
       </c>
       <c r="E5" t="s">
-        <v>109</v>
+        <v>53</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
-        <v>110</v>
+        <v>54</v>
       </c>
       <c r="C6" s="1">
         <v>0</v>
       </c>
       <c r="E6" t="s">
-        <v>111</v>
+        <v>55</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
-        <v>105</v>
+        <v>49</v>
       </c>
       <c r="C7" s="1">
         <v>0.8</v>
       </c>
       <c r="E7" t="s">
-        <v>112</v>
+        <v>56</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>106</v>
+        <v>50</v>
       </c>
       <c r="C8" s="1">
         <v>2</v>
       </c>
       <c r="E8" s="5" t="s">
-        <v>113</v>
+        <v>57</v>
       </c>
       <c r="I8" s="4" t="s">
-        <v>114</v>
+        <v>58</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
@@ -1675,13 +1522,13 @@
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" s="11" t="s">
-        <v>116</v>
+        <v>60</v>
       </c>
       <c r="B10" s="11"/>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
-        <v>118</v>
+        <v>62</v>
       </c>
       <c r="C11" s="1">
         <f>SUM(C3:C8)</f>
@@ -1690,7 +1537,7 @@
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
-        <v>117</v>
+        <v>61</v>
       </c>
       <c r="C12" s="1">
         <v>34.99</v>
@@ -1698,7 +1545,7 @@
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
-        <v>120</v>
+        <v>64</v>
       </c>
       <c r="C13" s="7">
         <f>C12-C11</f>
@@ -1707,7 +1554,7 @@
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
-        <v>119</v>
+        <v>63</v>
       </c>
       <c r="C14" s="6">
         <f>C13/C11</f>
@@ -1716,7 +1563,7 @@
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
-        <v>121</v>
+        <v>65</v>
       </c>
       <c r="C15" s="1">
         <v>8.3000000000000007</v>
@@ -1724,56 +1571,56 @@
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="4" t="s">
-        <v>122</v>
+        <v>66</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B18" t="s">
-        <v>123</v>
+        <v>67</v>
       </c>
       <c r="C18" s="1">
         <v>15.29</v>
       </c>
       <c r="E18" t="s">
-        <v>128</v>
+        <v>72</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B19" t="s">
-        <v>124</v>
+        <v>68</v>
       </c>
       <c r="C19" s="1">
         <v>38.950000000000003</v>
       </c>
       <c r="E19" t="s">
-        <v>127</v>
+        <v>71</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B20" t="s">
-        <v>125</v>
+        <v>69</v>
       </c>
       <c r="C20" s="1">
         <v>9</v>
       </c>
       <c r="E20" s="5" t="s">
-        <v>129</v>
+        <v>73</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B21" t="s">
-        <v>126</v>
+        <v>70</v>
       </c>
       <c r="C21" s="1">
         <v>20</v>
       </c>
       <c r="E21" t="s">
-        <v>131</v>
+        <v>75</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B23" t="s">
-        <v>130</v>
+        <v>74</v>
       </c>
       <c r="C23" s="2">
         <f>SUM(C18:C21)</f>
@@ -1782,17 +1629,17 @@
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" s="4" t="s">
-        <v>133</v>
+        <v>77</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B26" t="s">
-        <v>132</v>
+        <v>76</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B27" s="4" t="s">
-        <v>134</v>
+        <v>78</v>
       </c>
       <c r="C27" s="2">
         <f>C23+C15+C12</f>
@@ -1820,10 +1667,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:I33"/>
+  <dimension ref="A1:I17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I32" sqref="I32"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1848,99 +1695,99 @@
         <v>2</v>
       </c>
       <c r="D1" t="s">
-        <v>52</v>
+        <v>15</v>
       </c>
       <c r="E1" t="s">
-        <v>57</v>
+        <v>20</v>
       </c>
       <c r="F1" t="s">
-        <v>53</v>
+        <v>16</v>
       </c>
       <c r="G1" t="s">
-        <v>61</v>
+        <v>23</v>
       </c>
       <c r="I1" t="s">
-        <v>56</v>
+        <v>19</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="B2" t="s">
+        <v>91</v>
+      </c>
+      <c r="C2" t="s">
         <v>3</v>
       </c>
-      <c r="C2" t="s">
-        <v>4</v>
-      </c>
       <c r="D2">
-        <f>1000*A2</f>
-        <v>1000</v>
+        <f t="shared" ref="D2:D13" si="0">1000*A2</f>
+        <v>6000</v>
       </c>
       <c r="E2" s="1">
-        <v>25.12</v>
+        <v>0.86</v>
       </c>
       <c r="F2" s="1">
-        <f>E2*A2</f>
-        <v>25.12</v>
+        <f t="shared" ref="F2:F9" si="1">E2*A2</f>
+        <v>5.16</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>62</v>
+        <v>25</v>
       </c>
       <c r="I2" t="s">
-        <v>60</v>
+        <v>24</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3">
+        <v>1</v>
+      </c>
+      <c r="B3" t="s">
+        <v>89</v>
+      </c>
+      <c r="C3" t="s">
         <v>4</v>
       </c>
-      <c r="B3" t="s">
-        <v>43</v>
-      </c>
-      <c r="C3" t="s">
-        <v>5</v>
-      </c>
       <c r="D3">
-        <f t="shared" ref="D3:D29" si="0">1000*A3</f>
-        <v>4000</v>
+        <f t="shared" si="0"/>
+        <v>1000</v>
       </c>
       <c r="E3" s="1">
-        <v>0.05</v>
+        <v>7.0000000000000007E-2</v>
       </c>
       <c r="F3" s="1">
-        <f t="shared" ref="F3:F26" si="1">E3*A3</f>
-        <v>0.2</v>
+        <f t="shared" si="1"/>
+        <v>7.0000000000000007E-2</v>
       </c>
       <c r="G3" s="3"/>
       <c r="I3" t="s">
-        <v>65</v>
+        <v>26</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B4" t="s">
-        <v>44</v>
+        <v>90</v>
       </c>
       <c r="C4" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D4">
         <f t="shared" si="0"/>
-        <v>2000</v>
+        <v>1000</v>
       </c>
       <c r="E4" s="1">
-        <v>0.04</v>
+        <v>7.0000000000000007E-2</v>
       </c>
       <c r="F4" s="1">
         <f t="shared" si="1"/>
-        <v>0.08</v>
+        <v>7.0000000000000007E-2</v>
       </c>
       <c r="G4" s="3"/>
       <c r="I4" t="s">
-        <v>66</v>
+        <v>27</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
@@ -1948,25 +1795,27 @@
         <v>1</v>
       </c>
       <c r="B5" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C5" t="s">
-        <v>8</v>
+        <v>88</v>
       </c>
       <c r="D5">
         <f t="shared" si="0"/>
         <v>1000</v>
       </c>
       <c r="E5" s="1">
-        <v>0.03</v>
+        <v>1.85</v>
       </c>
       <c r="F5" s="1">
         <f t="shared" si="1"/>
-        <v>0.03</v>
-      </c>
-      <c r="G5" s="3"/>
+        <v>1.85</v>
+      </c>
+      <c r="G5" s="3" t="s">
+        <v>29</v>
+      </c>
       <c r="I5" t="s">
-        <v>67</v>
+        <v>28</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
@@ -1974,160 +1823,116 @@
         <v>1</v>
       </c>
       <c r="B6" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="C6" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="D6">
         <f t="shared" si="0"/>
         <v>1000</v>
       </c>
       <c r="E6" s="1">
-        <v>0.87</v>
+        <v>0.18</v>
       </c>
       <c r="F6" s="1">
         <f t="shared" si="1"/>
-        <v>0.87</v>
+        <v>0.18</v>
       </c>
       <c r="G6" s="3"/>
       <c r="I6" t="s">
-        <v>68</v>
+        <v>30</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="B7" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="C7" t="s">
         <v>11</v>
       </c>
       <c r="D7">
         <f t="shared" si="0"/>
-        <v>6000</v>
+        <v>2000</v>
       </c>
       <c r="E7" s="1">
-        <v>0.86</v>
+        <v>5.0000000000000001E-3</v>
       </c>
       <c r="F7" s="1">
         <f t="shared" si="1"/>
-        <v>5.16</v>
-      </c>
-      <c r="G7" s="3" t="s">
-        <v>64</v>
-      </c>
+        <v>0.01</v>
+      </c>
+      <c r="G7" s="3"/>
       <c r="I7" t="s">
-        <v>63</v>
+        <v>31</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B8" t="s">
-        <v>46</v>
+        <v>92</v>
       </c>
       <c r="C8" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="D8">
         <f t="shared" si="0"/>
-        <v>3000</v>
+        <v>2000</v>
       </c>
       <c r="E8" s="1">
-        <v>7.0000000000000007E-2</v>
+        <v>5.0000000000000001E-3</v>
       </c>
       <c r="F8" s="1">
         <f t="shared" si="1"/>
-        <v>0.21000000000000002</v>
+        <v>0.01</v>
       </c>
       <c r="G8" s="3"/>
       <c r="I8" t="s">
-        <v>69</v>
+        <v>32</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B9" t="s">
-        <v>47</v>
+        <v>14</v>
       </c>
       <c r="C9" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="D9">
         <f t="shared" si="0"/>
-        <v>3000</v>
+        <v>4000</v>
       </c>
       <c r="E9" s="1">
-        <v>7.0000000000000007E-2</v>
+        <v>5.0000000000000001E-3</v>
       </c>
       <c r="F9" s="1">
         <f t="shared" si="1"/>
-        <v>0.21000000000000002</v>
+        <v>0.02</v>
       </c>
       <c r="G9" s="3"/>
       <c r="I9" t="s">
-        <v>70</v>
+        <v>33</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A10">
-        <v>1</v>
-      </c>
-      <c r="B10" t="s">
-        <v>14</v>
-      </c>
-      <c r="C10" t="s">
-        <v>15</v>
-      </c>
-      <c r="D10">
-        <f t="shared" si="0"/>
-        <v>1000</v>
-      </c>
-      <c r="E10" s="1">
-        <v>0.38</v>
-      </c>
-      <c r="F10" s="1">
-        <f t="shared" si="1"/>
-        <v>0.38</v>
-      </c>
+      <c r="E10" s="1"/>
+      <c r="F10" s="1"/>
       <c r="G10" s="3"/>
-      <c r="I10" t="s">
-        <v>71</v>
-      </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A11">
-        <v>1</v>
-      </c>
-      <c r="B11" t="s">
-        <v>16</v>
-      </c>
-      <c r="C11" t="s">
-        <v>72</v>
-      </c>
-      <c r="D11">
-        <f t="shared" si="0"/>
-        <v>1000</v>
-      </c>
-      <c r="E11" s="1">
-        <v>1.85</v>
-      </c>
-      <c r="F11" s="1">
-        <f t="shared" si="1"/>
-        <v>1.85</v>
-      </c>
-      <c r="G11" s="3" t="s">
-        <v>74</v>
-      </c>
-      <c r="I11" t="s">
-        <v>73</v>
-      </c>
+      <c r="E11" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="F11" s="1"/>
+      <c r="G11" s="3"/>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12">
@@ -2136,23 +1941,19 @@
       <c r="B12" t="s">
         <v>17</v>
       </c>
-      <c r="C12" t="s">
-        <v>18</v>
-      </c>
       <c r="D12">
         <f t="shared" si="0"/>
         <v>1000</v>
       </c>
       <c r="E12" s="1">
-        <v>0.3</v>
+        <v>500</v>
       </c>
       <c r="F12" s="1">
-        <f t="shared" si="1"/>
-        <v>0.3</v>
-      </c>
-      <c r="G12" s="3"/>
-      <c r="I12" t="s">
-        <v>77</v>
+        <f>E12/D12</f>
+        <v>0.5</v>
+      </c>
+      <c r="G12" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
@@ -2160,25 +1961,21 @@
         <v>1</v>
       </c>
       <c r="B13" t="s">
-        <v>19</v>
-      </c>
-      <c r="C13" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="D13">
         <f t="shared" si="0"/>
         <v>1000</v>
       </c>
       <c r="E13" s="1">
-        <v>0.18</v>
+        <v>460</v>
       </c>
       <c r="F13" s="1">
-        <f t="shared" si="1"/>
-        <v>0.18</v>
-      </c>
-      <c r="G13" s="3"/>
-      <c r="I13" t="s">
-        <v>76</v>
+        <f t="shared" ref="F13:F14" si="2">E13/D13</f>
+        <v>0.46</v>
+      </c>
+      <c r="G13" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
@@ -2186,431 +1983,42 @@
         <v>1</v>
       </c>
       <c r="B14" t="s">
+        <v>34</v>
+      </c>
+      <c r="D14">
+        <v>1000</v>
+      </c>
+      <c r="E14" s="1">
+        <v>210</v>
+      </c>
+      <c r="F14" s="1">
+        <f t="shared" si="2"/>
+        <v>0.21</v>
+      </c>
+      <c r="G14" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="G15" s="3"/>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="E16" t="s">
         <v>21</v>
       </c>
-      <c r="C14" t="s">
+      <c r="F16" s="1">
+        <f>SUM(F2:F14)</f>
+        <v>8.5400000000000009</v>
+      </c>
+      <c r="I16" s="2"/>
+    </row>
+    <row r="17" spans="5:6" x14ac:dyDescent="0.25">
+      <c r="E17" t="s">
         <v>22</v>
       </c>
-      <c r="D14">
-        <f t="shared" si="0"/>
-        <v>1000</v>
-      </c>
-      <c r="E14" s="1">
-        <v>0.04</v>
-      </c>
-      <c r="F14" s="1">
-        <f t="shared" si="1"/>
-        <v>0.04</v>
-      </c>
-      <c r="G14" s="3"/>
-      <c r="I14" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A15">
-        <v>4</v>
-      </c>
-      <c r="B15" t="s">
-        <v>48</v>
-      </c>
-      <c r="C15" t="s">
-        <v>23</v>
-      </c>
-      <c r="D15">
-        <f t="shared" si="0"/>
-        <v>4000</v>
-      </c>
-      <c r="E15" s="1">
-        <v>5.0000000000000001E-3</v>
-      </c>
-      <c r="F15" s="1">
-        <f t="shared" si="1"/>
-        <v>0.02</v>
-      </c>
-      <c r="G15" s="3"/>
-      <c r="I15" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A16">
-        <v>4</v>
-      </c>
-      <c r="B16" t="s">
-        <v>49</v>
-      </c>
-      <c r="C16" t="s">
-        <v>24</v>
-      </c>
-      <c r="D16">
-        <f t="shared" si="0"/>
-        <v>4000</v>
-      </c>
-      <c r="E16" s="1">
-        <v>5.0000000000000001E-3</v>
-      </c>
-      <c r="F16" s="1">
-        <f t="shared" si="1"/>
-        <v>0.02</v>
-      </c>
-      <c r="G16" s="3"/>
-      <c r="I16" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A17">
-        <v>7</v>
-      </c>
-      <c r="B17" t="s">
-        <v>50</v>
-      </c>
-      <c r="C17" t="s">
-        <v>25</v>
-      </c>
-      <c r="D17">
-        <f t="shared" si="0"/>
-        <v>7000</v>
-      </c>
-      <c r="E17" s="1">
-        <v>5.0000000000000001E-3</v>
-      </c>
-      <c r="F17" s="1">
-        <f t="shared" si="1"/>
-        <v>3.5000000000000003E-2</v>
-      </c>
-      <c r="G17" s="3"/>
-      <c r="I17" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A18">
-        <v>1</v>
-      </c>
-      <c r="B18" t="s">
-        <v>26</v>
-      </c>
-      <c r="C18" t="s">
-        <v>27</v>
-      </c>
-      <c r="D18">
-        <f t="shared" si="0"/>
-        <v>1000</v>
-      </c>
-      <c r="E18" s="1">
-        <v>7.0000000000000001E-3</v>
-      </c>
-      <c r="F18" s="1">
-        <f t="shared" si="1"/>
-        <v>7.0000000000000001E-3</v>
-      </c>
-      <c r="G18" s="3"/>
-      <c r="I18" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A19">
-        <v>1</v>
-      </c>
-      <c r="B19" t="s">
-        <v>28</v>
-      </c>
-      <c r="C19" t="s">
-        <v>29</v>
-      </c>
-      <c r="D19">
-        <f t="shared" si="0"/>
-        <v>1000</v>
-      </c>
-      <c r="E19" s="1">
-        <v>5.0000000000000001E-3</v>
-      </c>
-      <c r="F19" s="1">
-        <f t="shared" si="1"/>
-        <v>5.0000000000000001E-3</v>
-      </c>
-      <c r="G19" s="3"/>
-      <c r="I19" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A20">
-        <v>1</v>
-      </c>
-      <c r="B20" t="s">
-        <v>30</v>
-      </c>
-      <c r="C20" t="s">
-        <v>31</v>
-      </c>
-      <c r="D20">
-        <f t="shared" si="0"/>
-        <v>1000</v>
-      </c>
-      <c r="E20" s="1">
-        <v>5.0000000000000001E-3</v>
-      </c>
-      <c r="F20" s="1">
-        <f t="shared" si="1"/>
-        <v>5.0000000000000001E-3</v>
-      </c>
-      <c r="G20" s="3"/>
-      <c r="I20" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A21">
-        <v>2</v>
-      </c>
-      <c r="B21" t="s">
-        <v>51</v>
-      </c>
-      <c r="C21" t="s">
-        <v>32</v>
-      </c>
-      <c r="D21">
-        <f t="shared" si="0"/>
-        <v>2000</v>
-      </c>
-      <c r="E21" s="1">
-        <v>5.0000000000000001E-3</v>
-      </c>
-      <c r="F21" s="1">
-        <f t="shared" si="1"/>
-        <v>0.01</v>
-      </c>
-      <c r="G21" s="3"/>
-      <c r="I21" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A22">
-        <v>1</v>
-      </c>
-      <c r="B22" t="s">
-        <v>33</v>
-      </c>
-      <c r="C22" t="s">
-        <v>34</v>
-      </c>
-      <c r="D22">
-        <f t="shared" si="0"/>
-        <v>1000</v>
-      </c>
-      <c r="E22" s="1">
-        <v>0.44</v>
-      </c>
-      <c r="F22" s="1">
-        <f t="shared" si="1"/>
-        <v>0.44</v>
-      </c>
-      <c r="G22" s="3"/>
-      <c r="I22" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A23">
-        <v>1</v>
-      </c>
-      <c r="B23" t="s">
-        <v>35</v>
-      </c>
-      <c r="C23" t="s">
-        <v>36</v>
-      </c>
-      <c r="D23">
-        <f t="shared" si="0"/>
-        <v>1000</v>
-      </c>
-      <c r="E23" s="1">
-        <v>0.09</v>
-      </c>
-      <c r="F23" s="1">
-        <f t="shared" si="1"/>
-        <v>0.09</v>
-      </c>
-      <c r="G23" s="3"/>
-      <c r="I23" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A24">
-        <v>1</v>
-      </c>
-      <c r="B24" t="s">
-        <v>37</v>
-      </c>
-      <c r="C24" t="s">
-        <v>38</v>
-      </c>
-      <c r="D24">
-        <f t="shared" si="0"/>
-        <v>1000</v>
-      </c>
-      <c r="E24" s="1">
-        <v>1.22</v>
-      </c>
-      <c r="F24" s="1">
-        <f t="shared" si="1"/>
-        <v>1.22</v>
-      </c>
-      <c r="G24" s="3"/>
-      <c r="I24" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A25">
-        <v>1</v>
-      </c>
-      <c r="B25" t="s">
-        <v>39</v>
-      </c>
-      <c r="C25" t="s">
-        <v>40</v>
-      </c>
-      <c r="D25">
-        <f t="shared" si="0"/>
-        <v>1000</v>
-      </c>
-      <c r="E25" s="1">
-        <v>1.73</v>
-      </c>
-      <c r="F25" s="1">
-        <f t="shared" si="1"/>
-        <v>1.73</v>
-      </c>
-      <c r="G25" s="3"/>
-      <c r="I25" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A26">
-        <v>1</v>
-      </c>
-      <c r="B26" t="s">
-        <v>41</v>
-      </c>
-      <c r="C26" t="s">
-        <v>42</v>
-      </c>
-      <c r="D26">
-        <f t="shared" si="0"/>
-        <v>1000</v>
-      </c>
-      <c r="E26" s="1">
-        <v>2.0299999999999998</v>
-      </c>
-      <c r="F26" s="1">
-        <f t="shared" si="1"/>
-        <v>2.0299999999999998</v>
-      </c>
-      <c r="G26" s="3"/>
-      <c r="I26" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="E27" s="1" t="s">
-        <v>99</v>
-      </c>
-      <c r="F27" s="1"/>
-      <c r="G27" s="3"/>
-    </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A28">
-        <v>1</v>
-      </c>
-      <c r="B28" t="s">
-        <v>54</v>
-      </c>
-      <c r="D28">
-        <f t="shared" si="0"/>
-        <v>1000</v>
-      </c>
-      <c r="E28" s="1">
-        <v>500</v>
-      </c>
-      <c r="F28" s="1">
-        <f>E28/D28</f>
-        <v>0.5</v>
-      </c>
-      <c r="G28" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A29">
-        <v>1</v>
-      </c>
-      <c r="B29" t="s">
-        <v>55</v>
-      </c>
-      <c r="D29">
-        <f t="shared" si="0"/>
-        <v>1000</v>
-      </c>
-      <c r="E29" s="1">
-        <v>870</v>
-      </c>
-      <c r="F29" s="1">
-        <f t="shared" ref="F29:F30" si="2">E29/D29</f>
-        <v>0.87</v>
-      </c>
-      <c r="G29" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A30">
-        <v>1</v>
-      </c>
-      <c r="B30" t="s">
-        <v>90</v>
-      </c>
-      <c r="D30">
-        <v>1000</v>
-      </c>
-      <c r="E30" s="1">
-        <v>250</v>
-      </c>
-      <c r="F30" s="1">
-        <f t="shared" si="2"/>
-        <v>0.25</v>
-      </c>
-      <c r="G30" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="G31" s="3"/>
-    </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="E32" t="s">
-        <v>58</v>
-      </c>
-      <c r="F32" s="1">
-        <f>SUM(F2:F30)</f>
-        <v>41.862000000000002</v>
-      </c>
-      <c r="I32" s="2"/>
-    </row>
-    <row r="33" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E33" t="s">
-        <v>59</v>
-      </c>
-      <c r="F33" s="2">
-        <f>F32*1.1</f>
-        <v>46.048200000000008</v>
+      <c r="F17" s="2">
+        <f>F16*1.1</f>
+        <v>9.3940000000000019</v>
       </c>
     </row>
   </sheetData>
@@ -2647,19 +2055,19 @@
         <v>2</v>
       </c>
       <c r="D1" t="s">
-        <v>52</v>
+        <v>15</v>
       </c>
       <c r="E1" t="s">
-        <v>57</v>
+        <v>20</v>
       </c>
       <c r="F1" t="s">
-        <v>53</v>
+        <v>16</v>
       </c>
       <c r="G1" t="s">
-        <v>61</v>
+        <v>23</v>
       </c>
       <c r="I1" t="s">
-        <v>56</v>
+        <v>19</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
@@ -2667,10 +2075,10 @@
         <v>5</v>
       </c>
       <c r="B2" t="s">
-        <v>92</v>
+        <v>36</v>
       </c>
       <c r="C2" t="s">
-        <v>11</v>
+        <v>3</v>
       </c>
       <c r="D2">
         <f t="shared" ref="D2:D12" si="0">1000*A2</f>
@@ -2684,10 +2092,10 @@
         <v>4.3</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>64</v>
+        <v>25</v>
       </c>
       <c r="I2" t="s">
-        <v>63</v>
+        <v>24</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
@@ -2695,10 +2103,10 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>46</v>
+        <v>12</v>
       </c>
       <c r="C3" t="s">
-        <v>12</v>
+        <v>4</v>
       </c>
       <c r="D3">
         <f t="shared" si="0"/>
@@ -2713,7 +2121,7 @@
       </c>
       <c r="G3" s="3"/>
       <c r="I3" t="s">
-        <v>69</v>
+        <v>26</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
@@ -2721,10 +2129,10 @@
         <v>1</v>
       </c>
       <c r="B4" t="s">
-        <v>47</v>
+        <v>13</v>
       </c>
       <c r="C4" t="s">
-        <v>13</v>
+        <v>5</v>
       </c>
       <c r="D4">
         <f t="shared" si="0"/>
@@ -2739,7 +2147,7 @@
       </c>
       <c r="G4" s="3"/>
       <c r="I4" t="s">
-        <v>70</v>
+        <v>27</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
@@ -2747,10 +2155,10 @@
         <v>1</v>
       </c>
       <c r="B5" t="s">
-        <v>19</v>
+        <v>7</v>
       </c>
       <c r="C5" t="s">
-        <v>20</v>
+        <v>8</v>
       </c>
       <c r="D5">
         <f t="shared" si="0"/>
@@ -2765,7 +2173,7 @@
       </c>
       <c r="G5" s="3"/>
       <c r="I5" t="s">
-        <v>76</v>
+        <v>30</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
@@ -2773,10 +2181,10 @@
         <v>2</v>
       </c>
       <c r="B6" t="s">
-        <v>93</v>
+        <v>37</v>
       </c>
       <c r="C6" t="s">
-        <v>23</v>
+        <v>9</v>
       </c>
       <c r="D6">
         <f t="shared" si="0"/>
@@ -2791,7 +2199,7 @@
       </c>
       <c r="G6" s="3"/>
       <c r="I6" t="s">
-        <v>78</v>
+        <v>31</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
@@ -2799,10 +2207,10 @@
         <v>2</v>
       </c>
       <c r="B7" t="s">
-        <v>94</v>
+        <v>38</v>
       </c>
       <c r="C7" t="s">
-        <v>24</v>
+        <v>10</v>
       </c>
       <c r="D7">
         <f t="shared" si="0"/>
@@ -2817,7 +2225,7 @@
       </c>
       <c r="G7" s="3"/>
       <c r="I7" t="s">
-        <v>79</v>
+        <v>32</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
@@ -2825,10 +2233,10 @@
         <v>2</v>
       </c>
       <c r="B8" t="s">
-        <v>95</v>
+        <v>39</v>
       </c>
       <c r="C8" t="s">
-        <v>25</v>
+        <v>11</v>
       </c>
       <c r="D8">
         <f t="shared" si="0"/>
@@ -2843,7 +2251,7 @@
       </c>
       <c r="G8" s="3"/>
       <c r="I8" t="s">
-        <v>80</v>
+        <v>33</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
@@ -2851,10 +2259,10 @@
         <v>2</v>
       </c>
       <c r="B9" t="s">
-        <v>96</v>
+        <v>40</v>
       </c>
       <c r="C9" t="s">
-        <v>97</v>
+        <v>41</v>
       </c>
       <c r="D9">
         <f t="shared" ref="D9" si="2">1000*A9</f>
@@ -2869,12 +2277,12 @@
       </c>
       <c r="G9" s="3"/>
       <c r="I9" t="s">
-        <v>98</v>
+        <v>42</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="E10" s="1" t="s">
-        <v>99</v>
+        <v>43</v>
       </c>
       <c r="F10" s="1"/>
       <c r="G10" s="3"/>
@@ -2884,7 +2292,7 @@
         <v>1</v>
       </c>
       <c r="B11" t="s">
-        <v>54</v>
+        <v>17</v>
       </c>
       <c r="D11">
         <f t="shared" si="0"/>
@@ -2898,7 +2306,7 @@
         <v>0.3</v>
       </c>
       <c r="G11" t="s">
-        <v>91</v>
+        <v>35</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
@@ -2906,7 +2314,7 @@
         <v>1</v>
       </c>
       <c r="B12" t="s">
-        <v>55</v>
+        <v>18</v>
       </c>
       <c r="D12">
         <f t="shared" si="0"/>
@@ -2920,7 +2328,7 @@
         <v>0.26</v>
       </c>
       <c r="G12" t="s">
-        <v>91</v>
+        <v>35</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
@@ -2928,7 +2336,7 @@
         <v>1</v>
       </c>
       <c r="B13" t="s">
-        <v>90</v>
+        <v>34</v>
       </c>
       <c r="D13">
         <v>1000</v>
@@ -2941,7 +2349,7 @@
         <v>0.14000000000000001</v>
       </c>
       <c r="G13" t="s">
-        <v>91</v>
+        <v>35</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
@@ -2949,7 +2357,7 @@
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="E15" t="s">
-        <v>58</v>
+        <v>21</v>
       </c>
       <c r="F15" s="1">
         <f>SUM(F2:F13)</f>
@@ -2958,7 +2366,7 @@
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="E16" t="s">
-        <v>59</v>
+        <v>22</v>
       </c>
       <c r="F16" s="2">
         <f>F15*1.1</f>

</xml_diff>

<commit_message>
More Hardware changes, both boards complete
</commit_message>
<xml_diff>
--- a/Hardware/Estimated Financials.xlsx
+++ b/Hardware/Estimated Financials.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Josh Johnson\Dropbox\ENGN4221\VeinCam2019\Hardware\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8AFD329F-6269-4957-BA19-AE974998079C}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{980263C4-0858-4297-8701-68241CBFDE3A}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="28110" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="RPi 3A+ Total BOM" sheetId="4" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="93">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="93">
   <si>
     <t>Qty</t>
   </si>
@@ -1186,10 +1186,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K26"/>
+  <dimension ref="A1:K27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C24" sqref="C24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1373,32 +1373,43 @@
         <v>73</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B22" t="s">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B21" t="s">
+        <v>70</v>
+      </c>
+      <c r="C21" s="1">
+        <v>20</v>
+      </c>
+      <c r="E21" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B23" t="s">
         <v>74</v>
       </c>
-      <c r="C22" s="2">
-        <f>SUM(C18:C20)</f>
-        <v>86.18</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A24" s="4" t="s">
+      <c r="C23" s="2">
+        <f>SUM(C18:C21)</f>
+        <v>106.18</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A25" s="4" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B25" t="s">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B26" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B26" s="4" t="s">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B27" s="4" t="s">
         <v>78</v>
       </c>
-      <c r="C26" s="2">
-        <f>C22+C15+C12</f>
-        <v>134.47</v>
+      <c r="C27" s="2">
+        <f>C23+C15+C12</f>
+        <v>154.47</v>
       </c>
     </row>
   </sheetData>
@@ -1421,7 +1432,7 @@
   <dimension ref="A1:I28"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C35" sqref="C35"/>
+      <selection activeCell="C36" sqref="C36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1670,7 +1681,7 @@
   <dimension ref="A1:I17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2030,8 +2041,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:I16"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
found possible IR filter suppliers
</commit_message>
<xml_diff>
--- a/Hardware/Estimated Financials.xlsx
+++ b/Hardware/Estimated Financials.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Josh Johnson\Dropbox\ENGN4221\VeinCam2019\Hardware\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD1952C6-8AD7-4482-B4BA-5E94D9626BB1}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A681C98-0729-4735-B8E7-D11116CB1A5F}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="93">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="158" uniqueCount="96">
   <si>
     <t>Qty</t>
   </si>
@@ -310,6 +310,15 @@
   </si>
   <si>
     <t>R7, R8</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Potential? </t>
+  </si>
+  <si>
+    <t>https://www.alibaba.com/product-detail/950-850-760-720-680nm-IR_60422676928.html?spm=a2700.7724838.2017115.399.3fcf3f7ctlOPXr</t>
+  </si>
+  <si>
+    <t>https://www.aliexpress.com/item/30mm-30-mm-Infrared-Infra-Red-IR-Filter-760nm-760/291484865.html?spm=2114.search0104.3.9.5440be1acELA94&amp;ws_ab_test=searchweb0_0,searchweb201602_8_10065_10068_10130_10547_319_317_10548_10696_453_10084_454_10083_10618_10307_537_536_10131_10132_10902_10133_10059_10884_10887_321_322_10103,searchweb201603_6,ppcSwitch_0&amp;algo_expid=69ddede1-8927-4705-bb6f-48a15eaabdc9-1&amp;algo_pvid=69ddede1-8927-4705-bb6f-48a15eaabdc9&amp;transAbTest=ae803_5</t>
   </si>
 </sst>
 </file>
@@ -1429,10 +1438,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:I28"/>
+  <dimension ref="A1:M28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+      <selection activeCell="M12" sqref="M12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1441,16 +1450,17 @@
     <col min="2" max="2" width="22" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="14.7109375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="5.42578125" customWidth="1"/>
+    <col min="12" max="12" width="10.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" s="9" t="s">
         <v>59</v>
       </c>
       <c r="B1" s="9"/>
       <c r="C1" s="9"/>
     </row>
-    <row r="2" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" s="9" t="s">
         <v>44</v>
       </c>
@@ -1463,7 +1473,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>45</v>
       </c>
@@ -1475,13 +1485,13 @@
         <v>52</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4" s="10" t="s">
         <v>46</v>
       </c>
       <c r="B4" s="10"/>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
         <v>48</v>
       </c>
@@ -1492,7 +1502,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
         <v>54</v>
       </c>
@@ -1503,7 +1513,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
         <v>49</v>
       </c>
@@ -1514,7 +1524,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>50</v>
       </c>
@@ -1527,17 +1537,26 @@
       <c r="I8" s="4" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="L8" t="s">
+        <v>93</v>
+      </c>
+      <c r="M8" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="C9" s="1"/>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="M9" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A10" s="11" t="s">
         <v>60</v>
       </c>
       <c r="B10" s="11"/>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
         <v>62</v>
       </c>
@@ -1546,7 +1565,7 @@
         <v>11.795999999999999</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
         <v>61</v>
       </c>
@@ -1554,7 +1573,7 @@
         <v>34.99</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
         <v>64</v>
       </c>
@@ -1563,7 +1582,7 @@
         <v>23.194000000000003</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
         <v>63</v>
       </c>
@@ -1572,7 +1591,7 @@
         <v>1.9662597490674809</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
         <v>65</v>
       </c>

</xml_diff>

<commit_message>
added potential suppliers for IR filter
</commit_message>
<xml_diff>
--- a/Hardware/Estimated Financials.xlsx
+++ b/Hardware/Estimated Financials.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Josh Johnson\Dropbox\ENGN4221\VeinCam2019\Hardware\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A681C98-0729-4735-B8E7-D11116CB1A5F}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F70CE78-568B-4184-80D0-C7874DD92385}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -312,13 +312,13 @@
     <t>R7, R8</t>
   </si>
   <si>
-    <t xml:space="preserve">Potential? </t>
-  </si>
-  <si>
     <t>https://www.alibaba.com/product-detail/950-850-760-720-680nm-IR_60422676928.html?spm=a2700.7724838.2017115.399.3fcf3f7ctlOPXr</t>
   </si>
   <si>
     <t>https://www.aliexpress.com/item/30mm-30-mm-Infrared-Infra-Red-IR-Filter-760nm-760/291484865.html?spm=2114.search0104.3.9.5440be1acELA94&amp;ws_ab_test=searchweb0_0,searchweb201602_8_10065_10068_10130_10547_319_317_10548_10696_453_10084_454_10083_10618_10307_537_536_10131_10132_10902_10133_10059_10884_10887_321_322_10103,searchweb201603_6,ppcSwitch_0&amp;algo_expid=69ddede1-8927-4705-bb6f-48a15eaabdc9-1&amp;algo_pvid=69ddede1-8927-4705-bb6f-48a15eaabdc9&amp;transAbTest=ae803_5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Potential Supplier? </t>
   </si>
 </sst>
 </file>
@@ -1441,7 +1441,7 @@
   <dimension ref="A1:M28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M12" sqref="M12"/>
+      <selection activeCell="L9" sqref="L9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1538,16 +1538,16 @@
         <v>58</v>
       </c>
       <c r="L8" t="s">
+        <v>95</v>
+      </c>
+      <c r="M8" t="s">
         <v>93</v>
-      </c>
-      <c r="M8" t="s">
-        <v>94</v>
       </c>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="C9" s="1"/>
       <c r="M9" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Added 3d Models + hardware readme
</commit_message>
<xml_diff>
--- a/Hardware/Estimated Financials.xlsx
+++ b/Hardware/Estimated Financials.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Josh Johnson\Dropbox\ENGN4221\VeinCam2019\Hardware\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jonno\Dropbox\ENGN4221\VeinCam2019\Hardware\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3DDBC314-1CA9-4204-8AE3-C305D7DC9109}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5901C726-B56C-4904-B051-E9937322521E}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13276" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="RPi 3A+ Total BOM" sheetId="4" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="158" uniqueCount="96">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="159" uniqueCount="97">
   <si>
     <t>Qty</t>
   </si>
@@ -319,6 +319,9 @@
   </si>
   <si>
     <t xml:space="preserve">Potential Supplier? </t>
+  </si>
+  <si>
+    <t>Screws: https://www.ebay.com.au/itm/M2-5-3-60mm-Pan-Head-Phillips-Screws-Machine-Screws-Bolts-G304-Stainless-Steel/273041450256?hash=item3f9289e510:m:mb2_CJinIu0oHCrNUTmbEdw</t>
   </si>
 </sst>
 </file>
@@ -1197,24 +1200,24 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K27"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C24" sqref="C24"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J14" sqref="J14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="2" max="2" width="22.140625" customWidth="1"/>
-    <col min="3" max="3" width="14.42578125" customWidth="1"/>
+    <col min="2" max="2" width="22.1328125" customWidth="1"/>
+    <col min="3" max="3" width="14.3984375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A1" s="9" t="s">
         <v>59</v>
       </c>
       <c r="B1" s="9"/>
       <c r="C1" s="9"/>
     </row>
-    <row r="2" spans="1:11" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" ht="30.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A2" s="9" t="s">
         <v>44</v>
       </c>
@@ -1227,7 +1230,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
         <v>45</v>
       </c>
@@ -1239,13 +1242,13 @@
         <v>87</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A4" s="10" t="s">
         <v>46</v>
       </c>
       <c r="B4" s="10"/>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.45">
       <c r="B5" t="s">
         <v>80</v>
       </c>
@@ -1259,7 +1262,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.45">
       <c r="B6" t="s">
         <v>79</v>
       </c>
@@ -1270,7 +1273,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.45">
       <c r="B7" t="s">
         <v>83</v>
       </c>
@@ -1280,8 +1283,11 @@
       <c r="E7" t="s">
         <v>84</v>
       </c>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="H7" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A8" t="s">
         <v>50</v>
       </c>
@@ -1292,16 +1298,16 @@
         <v>57</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.45">
       <c r="C9" s="1"/>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A10" s="11" t="s">
         <v>60</v>
       </c>
       <c r="B10" s="11"/>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.45">
       <c r="B11" t="s">
         <v>62</v>
       </c>
@@ -1310,7 +1316,7 @@
         <v>14.194000000000003</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.45">
       <c r="B12" t="s">
         <v>61</v>
       </c>
@@ -1318,7 +1324,7 @@
         <v>39.99</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.45">
       <c r="B13" t="s">
         <v>64</v>
       </c>
@@ -1327,7 +1333,7 @@
         <v>25.795999999999999</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.45">
       <c r="B14" t="s">
         <v>63</v>
       </c>
@@ -1336,7 +1342,7 @@
         <v>1.817387628575454</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.45">
       <c r="B15" t="s">
         <v>65</v>
       </c>
@@ -1344,12 +1350,12 @@
         <v>8.3000000000000007</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A17" s="4" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.45">
       <c r="B18" t="s">
         <v>85</v>
       </c>
@@ -1360,7 +1366,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.45">
       <c r="B19" t="s">
         <v>68</v>
       </c>
@@ -1371,7 +1377,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.45">
       <c r="B20" t="s">
         <v>69</v>
       </c>
@@ -1382,7 +1388,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.45">
       <c r="B21" t="s">
         <v>70</v>
       </c>
@@ -1393,7 +1399,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.45">
       <c r="B23" t="s">
         <v>74</v>
       </c>
@@ -1402,17 +1408,17 @@
         <v>106.18</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A25" s="4" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.45">
       <c r="B26" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.45">
       <c r="B27" s="4" t="s">
         <v>78</v>
       </c>
@@ -1440,27 +1446,27 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:M28"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="N15" sqref="N15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="9.85546875" customWidth="1"/>
+    <col min="1" max="1" width="9.86328125" customWidth="1"/>
     <col min="2" max="2" width="22" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="5.42578125" customWidth="1"/>
-    <col min="12" max="12" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.73046875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="5.3984375" customWidth="1"/>
+    <col min="12" max="12" width="10.59765625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A1" s="9" t="s">
         <v>59</v>
       </c>
       <c r="B1" s="9"/>
       <c r="C1" s="9"/>
     </row>
-    <row r="2" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:13" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A2" s="9" t="s">
         <v>44</v>
       </c>
@@ -1473,7 +1479,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
         <v>45</v>
       </c>
@@ -1485,13 +1491,13 @@
         <v>52</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A4" s="10" t="s">
         <v>46</v>
       </c>
       <c r="B4" s="10"/>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.45">
       <c r="B5" t="s">
         <v>48</v>
       </c>
@@ -1502,7 +1508,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.45">
       <c r="B6" t="s">
         <v>54</v>
       </c>
@@ -1513,7 +1519,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.45">
       <c r="B7" t="s">
         <v>49</v>
       </c>
@@ -1524,7 +1530,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A8" t="s">
         <v>50</v>
       </c>
@@ -1544,19 +1550,19 @@
         <v>93</v>
       </c>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.45">
       <c r="C9" s="1"/>
       <c r="M9" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A10" s="11" t="s">
         <v>60</v>
       </c>
       <c r="B10" s="11"/>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.45">
       <c r="B11" t="s">
         <v>62</v>
       </c>
@@ -1565,7 +1571,7 @@
         <v>11.795999999999999</v>
       </c>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.45">
       <c r="B12" t="s">
         <v>61</v>
       </c>
@@ -1573,7 +1579,7 @@
         <v>34.99</v>
       </c>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.45">
       <c r="B13" t="s">
         <v>64</v>
       </c>
@@ -1582,7 +1588,7 @@
         <v>23.194000000000003</v>
       </c>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.45">
       <c r="B14" t="s">
         <v>63</v>
       </c>
@@ -1591,7 +1597,7 @@
         <v>1.9662597490674809</v>
       </c>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.45">
       <c r="B15" t="s">
         <v>65</v>
       </c>
@@ -1599,12 +1605,12 @@
         <v>8.3000000000000007</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A17" s="4" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.45">
       <c r="B18" t="s">
         <v>67</v>
       </c>
@@ -1615,7 +1621,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.45">
       <c r="B19" t="s">
         <v>68</v>
       </c>
@@ -1626,7 +1632,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.45">
       <c r="B20" t="s">
         <v>69</v>
       </c>
@@ -1637,7 +1643,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.45">
       <c r="B21" t="s">
         <v>70</v>
       </c>
@@ -1648,7 +1654,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.45">
       <c r="B23" t="s">
         <v>74</v>
       </c>
@@ -1657,17 +1663,17 @@
         <v>83.240000000000009</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A25" s="4" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.45">
       <c r="B26" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.45">
       <c r="B27" s="4" t="s">
         <v>78</v>
       </c>
@@ -1676,7 +1682,7 @@
         <v>126.53</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.45">
       <c r="C28" s="2"/>
     </row>
   </sheetData>
@@ -1703,18 +1709,18 @@
       <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="2" max="2" width="29.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="29.73046875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="22" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="27.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.73046875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="27.265625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="14" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="19.5703125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="19.59765625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.1328125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1740,7 +1746,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A2">
         <v>6</v>
       </c>
@@ -1768,7 +1774,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A3">
         <v>1</v>
       </c>
@@ -1794,7 +1800,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A4">
         <v>1</v>
       </c>
@@ -1820,7 +1826,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A5">
         <v>1</v>
       </c>
@@ -1848,7 +1854,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A6">
         <v>1</v>
       </c>
@@ -1874,7 +1880,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A7">
         <v>2</v>
       </c>
@@ -1900,7 +1906,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A8">
         <v>2</v>
       </c>
@@ -1926,7 +1932,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A9">
         <v>4</v>
       </c>
@@ -1952,19 +1958,19 @@
         <v>33</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.45">
       <c r="E10" s="1"/>
       <c r="F10" s="1"/>
       <c r="G10" s="3"/>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.45">
       <c r="E11" s="1" t="s">
         <v>43</v>
       </c>
       <c r="F11" s="1"/>
       <c r="G11" s="3"/>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A12">
         <v>1</v>
       </c>
@@ -1986,7 +1992,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A13">
         <v>1</v>
       </c>
@@ -2008,7 +2014,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A14">
         <v>1</v>
       </c>
@@ -2029,10 +2035,10 @@
         <v>35</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.45">
       <c r="G15" s="3"/>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.45">
       <c r="E16" t="s">
         <v>21</v>
       </c>
@@ -2042,7 +2048,7 @@
       </c>
       <c r="I16" s="2"/>
     </row>
-    <row r="17" spans="5:6" x14ac:dyDescent="0.25">
+    <row r="17" spans="5:6" x14ac:dyDescent="0.45">
       <c r="E17" t="s">
         <v>22</v>
       </c>
@@ -2064,17 +2070,17 @@
       <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="2" max="2" width="29.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="27.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="29.73046875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.3984375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.73046875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="27.265625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="14" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="17.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="17.3984375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2100,7 +2106,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A2">
         <v>5</v>
       </c>
@@ -2128,7 +2134,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A3">
         <v>1</v>
       </c>
@@ -2154,7 +2160,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A4">
         <v>1</v>
       </c>
@@ -2180,7 +2186,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A5">
         <v>1</v>
       </c>
@@ -2206,7 +2212,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A6">
         <v>2</v>
       </c>
@@ -2232,7 +2238,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A7">
         <v>2</v>
       </c>
@@ -2258,7 +2264,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A8">
         <v>2</v>
       </c>
@@ -2284,7 +2290,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A9">
         <v>2</v>
       </c>
@@ -2310,14 +2316,14 @@
         <v>42</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.45">
       <c r="E10" s="1" t="s">
         <v>43</v>
       </c>
       <c r="F10" s="1"/>
       <c r="G10" s="3"/>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A11">
         <v>1</v>
       </c>
@@ -2339,7 +2345,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A12">
         <v>1</v>
       </c>
@@ -2361,7 +2367,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A13">
         <v>1</v>
       </c>
@@ -2382,10 +2388,10 @@
         <v>35</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.45">
       <c r="G14" s="3"/>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.45">
       <c r="E15" t="s">
         <v>21</v>
       </c>
@@ -2394,7 +2400,7 @@
         <v>5.3599999999999985</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.45">
       <c r="E16" t="s">
         <v>22</v>
       </c>

</xml_diff>

<commit_message>
Changed pricing details and added links for mounting hardware.
</commit_message>
<xml_diff>
--- a/Hardware/Estimated Financials.xlsx
+++ b/Hardware/Estimated Financials.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jonno\Dropbox\ENGN4221\VeinCam2019\Hardware\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Josh Johnson\Dropbox\ENGN4221\VeinCam2019\Hardware\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5901C726-B56C-4904-B051-E9937322521E}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{422B842E-C8B3-47B2-B46F-F64FA45D2A8D}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13276" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="RPi 3A+ Total BOM" sheetId="4" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="159" uniqueCount="97">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="194" uniqueCount="103">
   <si>
     <t>Qty</t>
   </si>
@@ -57,9 +57,6 @@
     <t>Q1</t>
   </si>
   <si>
-    <t>BSD235N</t>
-  </si>
-  <si>
     <t>3R3</t>
   </si>
   <si>
@@ -120,12 +117,6 @@
     <t>https://www.digikey.com.au/product-detail/en/sullins-connector-solutions/PPTC202LFBN-RC/S6104-ND/807240</t>
   </si>
   <si>
-    <t>&lt;$0.20 ea from China</t>
-  </si>
-  <si>
-    <t>https://www.digikey.com.au/product-detail/en/infineon-technologies/BSD235NH6327XTSA1/BSD235NH6327XTSA1CT-ND/3196626</t>
-  </si>
-  <si>
     <t>https://www.digikey.com.au/product-detail/en/te-connectivity-passive-product/CRGCQ0603J3R3/A130076CT-ND/8577908</t>
   </si>
   <si>
@@ -177,12 +168,6 @@
     <t>Per Unit Cost (Quantity 1000)</t>
   </si>
   <si>
-    <t>Case</t>
-  </si>
-  <si>
-    <t>Labour to modify</t>
-  </si>
-  <si>
     <t>IR Filter</t>
   </si>
   <si>
@@ -192,24 +177,9 @@
     <t>See VeinCamHatZero Sheet</t>
   </si>
   <si>
-    <t>https://www.aliexpress.com/item/Raspberry-Pi-Zero-Case-Raspberry-Pi-Zero-W-Official-Case-ABS-Box-Enclosure-Cover-Shell-for/32843464423.html</t>
-  </si>
-  <si>
     <t>Camera FFC</t>
   </si>
   <si>
-    <t>Included with above</t>
-  </si>
-  <si>
-    <t>Unkown, based on $600 cost for 1000</t>
-  </si>
-  <si>
-    <t>http://www.camera-lensfilters.com/</t>
-  </si>
-  <si>
-    <t>NEED TO GET EXACT LINK</t>
-  </si>
-  <si>
     <t>Bare Bones RPi Zero w/ offical case</t>
   </si>
   <si>
@@ -276,18 +246,9 @@
     <t>Acrylic</t>
   </si>
   <si>
-    <t>https://www.clarkrubber.com.au/acrylic-sheet-clear</t>
-  </si>
-  <si>
-    <t>Bulk pricing likely better elsewhere</t>
-  </si>
-  <si>
     <t>Mounting hardware</t>
   </si>
   <si>
-    <t>TBD - will be various</t>
-  </si>
-  <si>
     <t>Raspberry Pi 3 A +</t>
   </si>
   <si>
@@ -312,16 +273,73 @@
     <t>R7, R8</t>
   </si>
   <si>
-    <t>https://www.alibaba.com/product-detail/950-850-760-720-680nm-IR_60422676928.html?spm=a2700.7724838.2017115.399.3fcf3f7ctlOPXr</t>
-  </si>
-  <si>
-    <t>https://www.aliexpress.com/item/30mm-30-mm-Infrared-Infra-Red-IR-Filter-760nm-760/291484865.html?spm=2114.search0104.3.9.5440be1acELA94&amp;ws_ab_test=searchweb0_0,searchweb201602_8_10065_10068_10130_10547_319_317_10548_10696_453_10084_454_10083_10618_10307_537_536_10131_10132_10902_10133_10059_10884_10887_321_322_10103,searchweb201603_6,ppcSwitch_0&amp;algo_expid=69ddede1-8927-4705-bb6f-48a15eaabdc9-1&amp;algo_pvid=69ddede1-8927-4705-bb6f-48a15eaabdc9&amp;transAbTest=ae803_5</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Potential Supplier? </t>
-  </si>
-  <si>
-    <t>Screws: https://www.ebay.com.au/itm/M2-5-3-60mm-Pan-Head-Phillips-Screws-Machine-Screws-Bolts-G304-Stainless-Steel/273041450256?hash=item3f9289e510:m:mb2_CJinIu0oHCrNUTmbEdw</t>
+    <t>Generic Item - 3mm Acrylic</t>
+  </si>
+  <si>
+    <t>TBD</t>
+  </si>
+  <si>
+    <t>Mounting Hardware</t>
+  </si>
+  <si>
+    <t>Quantity</t>
+  </si>
+  <si>
+    <t>Cost ea</t>
+  </si>
+  <si>
+    <t>Cost total</t>
+  </si>
+  <si>
+    <t>M2.5 * 28mm Screw</t>
+  </si>
+  <si>
+    <t>M3 * 11mm Spacer</t>
+  </si>
+  <si>
+    <t>M3 * 3mm Spacer</t>
+  </si>
+  <si>
+    <t>M2.5 Nut</t>
+  </si>
+  <si>
+    <t>M2 Nut</t>
+  </si>
+  <si>
+    <t>M2 * 4mm Screw</t>
+  </si>
+  <si>
+    <t>Total Cost:</t>
+  </si>
+  <si>
+    <t>https://www.ebay.com.au/itm/M2-5-3-60mm-Pan-Head-Phillips-Screws-Machine-Screws-Bolts-G304-Stainless-Steel/273041450256?ssPageName=STRK%3AMEBIDX%3AIT&amp;var=572285006604&amp;_trksid=p2060353.m2749.l2649</t>
+  </si>
+  <si>
+    <t>Look in this direction -&gt;</t>
+  </si>
+  <si>
+    <t>https://www.aliexpress.com/item/100Pcs-50pcs-m1-m1-2-m1-4-m1-6-M2-M2-5-M3-M4-DIN7985-GB818/32948746653.html?spm=a2g0s.9042311.0.0.1f924c4dMJUkZe</t>
+  </si>
+  <si>
+    <t>https://www.aliexpress.com/item/50pcs-M3-M4-M5-M6-M8-White-Nylon-ABS-Non-Threaded-Spacer-Round-Hollow-Standoff-Washer/32868508973.html?spm=a2g0s.9042311.0.0.1f924c4dMJUkZe</t>
+  </si>
+  <si>
+    <t>https://www.aliexpress.com/item/50Pcs-DIN934-M2-M2-5-M3-M4-M5-M6-M8-304-Stainless-Steel-Metric-Thread-Hex/32958861614.html?spm=a2g0s.9042311.0.0.1f924c4dMJUkZe</t>
+  </si>
+  <si>
+    <t>$0.02 from China</t>
+  </si>
+  <si>
+    <t>NTJD4001N</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com.au/product-detail/en/on-semiconductor/NTJD4001NT1G/NTJD4001NT1GOSCT-ND/687105</t>
+  </si>
+  <si>
+    <t>China Price' shown</t>
+  </si>
+  <si>
+    <t>Ebay / may already own</t>
   </si>
 </sst>
 </file>
@@ -331,7 +349,7 @@
   <numFmts count="1">
     <numFmt numFmtId="44" formatCode="_-&quot;$&quot;* #,##0.00_-;\-&quot;$&quot;* #,##0.00_-;_-&quot;$&quot;* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
-  <fonts count="19" x14ac:knownFonts="1">
+  <fonts count="20" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -470,6 +488,12 @@
       <u/>
       <sz val="11"/>
       <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -819,7 +843,7 @@
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -840,6 +864,8 @@
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="44" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="1" quotePrefix="1" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="45">
     <cellStyle name="20% - Accent1" xfId="21" builtinId="30" customBuiltin="1"/>
@@ -1198,229 +1224,345 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K27"/>
+  <dimension ref="A1:O27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J14" sqref="J14"/>
+      <selection activeCell="E22" sqref="E22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="22.1328125" customWidth="1"/>
-    <col min="3" max="3" width="14.3984375" customWidth="1"/>
+    <col min="2" max="2" width="22.140625" customWidth="1"/>
+    <col min="3" max="3" width="14.42578125" customWidth="1"/>
+    <col min="10" max="10" width="18.85546875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="9.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A1" s="9" t="s">
-        <v>59</v>
+        <v>49</v>
       </c>
       <c r="B1" s="9"/>
       <c r="C1" s="9"/>
     </row>
-    <row r="2" spans="1:11" ht="30.75" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:15" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="9" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="B2" s="9"/>
       <c r="C2" s="8" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="D2" s="4"/>
       <c r="E2" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.45">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="C3" s="2">
         <f>'VeinCamHat BOM'!F17</f>
-        <v>9.3940000000000019</v>
+        <v>7.5680000000000005</v>
       </c>
       <c r="E3" t="s">
+        <v>74</v>
+      </c>
+      <c r="J3" t="s">
+        <v>82</v>
+      </c>
+      <c r="K3" t="s">
+        <v>83</v>
+      </c>
+      <c r="L3" t="s">
+        <v>84</v>
+      </c>
+      <c r="M3" t="s">
+        <v>85</v>
+      </c>
+      <c r="O3" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A4" s="10" t="s">
+        <v>43</v>
+      </c>
+      <c r="B4" s="10"/>
+      <c r="J4" t="s">
+        <v>86</v>
+      </c>
+      <c r="K4">
+        <v>4</v>
+      </c>
+      <c r="L4" s="1">
+        <v>0.107</v>
+      </c>
+      <c r="M4" s="1">
+        <f>L4*K4</f>
+        <v>0.42799999999999999</v>
+      </c>
+      <c r="O4" s="5" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B5" t="s">
+        <v>70</v>
+      </c>
+      <c r="C5" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="E5" t="s">
+        <v>80</v>
+      </c>
+      <c r="J5" t="s">
         <v>87</v>
       </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.45">
-      <c r="A4" s="10" t="s">
-        <v>46</v>
-      </c>
-      <c r="B4" s="10"/>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.45">
-      <c r="B5" t="s">
-        <v>80</v>
-      </c>
-      <c r="C5" s="1">
-        <v>1</v>
-      </c>
-      <c r="E5" t="s">
+      <c r="K5">
+        <v>4</v>
+      </c>
+      <c r="L5" s="1">
+        <v>5.8000000000000003E-2</v>
+      </c>
+      <c r="M5" s="1">
+        <f t="shared" ref="M5:M9" si="0">L5*K5</f>
+        <v>0.23200000000000001</v>
+      </c>
+      <c r="O5" s="5" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B6" t="s">
+        <v>69</v>
+      </c>
+      <c r="C6" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="E6" t="s">
         <v>81</v>
       </c>
-      <c r="K5" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.45">
-      <c r="B6" t="s">
-        <v>79</v>
-      </c>
-      <c r="C6" s="1">
-        <v>0.8</v>
-      </c>
-      <c r="E6" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="J6" t="s">
+        <v>88</v>
+      </c>
+      <c r="K6">
+        <v>8</v>
+      </c>
+      <c r="L6" s="1">
+        <v>5.8000000000000003E-2</v>
+      </c>
+      <c r="M6" s="1">
+        <f t="shared" si="0"/>
+        <v>0.46400000000000002</v>
+      </c>
+      <c r="O6" s="5" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
-        <v>83</v>
+        <v>71</v>
       </c>
       <c r="C7" s="1">
-        <v>1</v>
+        <f>M10</f>
+        <v>1.4880000000000004</v>
       </c>
       <c r="E7" t="s">
-        <v>84</v>
-      </c>
-      <c r="H7" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.45">
+        <v>94</v>
+      </c>
+      <c r="J7" t="s">
+        <v>91</v>
+      </c>
+      <c r="K7">
+        <v>4</v>
+      </c>
+      <c r="L7" s="1">
+        <v>2.5000000000000001E-2</v>
+      </c>
+      <c r="M7" s="1">
+        <f t="shared" si="0"/>
+        <v>0.1</v>
+      </c>
+      <c r="O7" s="5" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="C8" s="1">
         <v>2</v>
       </c>
-      <c r="E8" s="5" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="E8" s="12" t="s">
+        <v>81</v>
+      </c>
+      <c r="J8" t="s">
+        <v>89</v>
+      </c>
+      <c r="K8">
+        <v>4</v>
+      </c>
+      <c r="L8" s="1">
+        <v>3.3000000000000002E-2</v>
+      </c>
+      <c r="M8" s="1">
+        <f t="shared" si="0"/>
+        <v>0.13200000000000001</v>
+      </c>
+      <c r="O8" s="5" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
       <c r="C9" s="1"/>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="J9" t="s">
+        <v>90</v>
+      </c>
+      <c r="K9">
+        <v>4</v>
+      </c>
+      <c r="L9" s="1">
+        <v>3.3000000000000002E-2</v>
+      </c>
+      <c r="M9" s="1">
+        <f t="shared" si="0"/>
+        <v>0.13200000000000001</v>
+      </c>
+      <c r="O9" s="5" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A10" s="11" t="s">
-        <v>60</v>
+        <v>50</v>
       </c>
       <c r="B10" s="11"/>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="L10" t="s">
+        <v>92</v>
+      </c>
+      <c r="M10" s="1">
+        <f>SUM(M4:M9)</f>
+        <v>1.4880000000000004</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
-        <v>62</v>
+        <v>52</v>
       </c>
       <c r="C11" s="1">
         <f>SUM(C3:C8)</f>
-        <v>14.194000000000003</v>
-      </c>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.45">
+        <v>12.056000000000001</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
-        <v>61</v>
+        <v>51</v>
       </c>
       <c r="C12" s="1">
         <v>39.99</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
-        <v>64</v>
+        <v>54</v>
       </c>
       <c r="C13" s="7">
         <f>C12-C11</f>
-        <v>25.795999999999999</v>
-      </c>
-    </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.45">
+        <v>27.934000000000001</v>
+      </c>
+    </row>
+    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
-        <v>63</v>
+        <v>53</v>
       </c>
       <c r="C14" s="6">
         <f>C13/C11</f>
-        <v>1.817387628575454</v>
-      </c>
-    </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.45">
+        <v>2.3170205706702056</v>
+      </c>
+    </row>
+    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
-        <v>65</v>
+        <v>55</v>
       </c>
       <c r="C15" s="1">
         <v>8.3000000000000007</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="4" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.45">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B18" t="s">
-        <v>85</v>
+        <v>72</v>
       </c>
       <c r="C18" s="1">
         <v>38.229999999999997</v>
       </c>
       <c r="E18" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.45">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B19" t="s">
-        <v>68</v>
+        <v>58</v>
       </c>
       <c r="C19" s="1">
         <v>38.950000000000003</v>
       </c>
       <c r="E19" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.45">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B20" t="s">
-        <v>69</v>
+        <v>59</v>
       </c>
       <c r="C20" s="1">
         <v>9</v>
       </c>
       <c r="E20" s="5" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.45">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B21" t="s">
-        <v>70</v>
+        <v>60</v>
       </c>
       <c r="C21" s="1">
         <v>20</v>
       </c>
       <c r="E21" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.45">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B23" t="s">
-        <v>74</v>
+        <v>64</v>
       </c>
       <c r="C23" s="2">
         <f>SUM(C18:C21)</f>
         <v>106.18</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" s="4" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.45">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B26" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.45">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B27" s="4" t="s">
-        <v>78</v>
+        <v>68</v>
       </c>
       <c r="C27" s="2">
         <f>C23+C15+C12</f>
@@ -1435,8 +1577,13 @@
     <mergeCell ref="A10:B10"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="E8" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
-    <hyperlink ref="E20" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
+    <hyperlink ref="E20" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
+    <hyperlink ref="O4" r:id="rId2" xr:uid="{15831DEE-A6A1-4D03-BA9B-B20F6C6807D4}"/>
+    <hyperlink ref="O7" r:id="rId3" xr:uid="{9B98D2E0-877B-4C9B-8F40-18E6E7ADCCEE}"/>
+    <hyperlink ref="O5" r:id="rId4" xr:uid="{CA668A5A-75C5-4964-9717-E58376AF80AA}"/>
+    <hyperlink ref="O6" r:id="rId5" xr:uid="{0FA79612-40E9-44C6-A6A1-0DCBDF1B8A6B}"/>
+    <hyperlink ref="O8" r:id="rId6" xr:uid="{B27C6BF6-FA47-4A12-8E8E-E3982DFB9EEB}"/>
+    <hyperlink ref="O9" r:id="rId7" xr:uid="{5E636539-9201-4464-A8E8-CA351037BED5}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1444,260 +1591,381 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:M28"/>
+  <dimension ref="A1:N29"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="N15" sqref="N15"/>
+      <selection activeCell="F38" sqref="F38"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.86328125" customWidth="1"/>
+    <col min="1" max="1" width="9.85546875" customWidth="1"/>
     <col min="2" max="2" width="22" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.73046875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="5.3984375" customWidth="1"/>
-    <col min="12" max="12" width="10.59765625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="5.42578125" customWidth="1"/>
+    <col min="12" max="12" width="10.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1" s="9" t="s">
-        <v>59</v>
+        <v>49</v>
       </c>
       <c r="B1" s="9"/>
       <c r="C1" s="9"/>
     </row>
-    <row r="2" spans="1:13" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:14" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" s="9" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="B2" s="9"/>
       <c r="C2" s="8" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="D2" s="4"/>
       <c r="E2" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.45">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="C3" s="2">
         <f>'VeinCamHatZero BOM'!F16</f>
         <v>5.895999999999999</v>
       </c>
       <c r="E3" t="s">
+        <v>47</v>
+      </c>
+      <c r="I3" t="s">
+        <v>82</v>
+      </c>
+      <c r="J3" t="s">
+        <v>83</v>
+      </c>
+      <c r="K3" t="s">
+        <v>84</v>
+      </c>
+      <c r="L3" t="s">
+        <v>85</v>
+      </c>
+      <c r="N3" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A4" s="10" t="s">
+        <v>43</v>
+      </c>
+      <c r="B4" s="10"/>
+      <c r="I4" t="s">
+        <v>86</v>
+      </c>
+      <c r="J4">
+        <v>4</v>
+      </c>
+      <c r="K4" s="1">
+        <v>0.107</v>
+      </c>
+      <c r="L4" s="1">
+        <f>K4*J4</f>
+        <v>0.42799999999999999</v>
+      </c>
+      <c r="N4" s="5" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B5" t="s">
+        <v>70</v>
+      </c>
+      <c r="C5" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="E5" t="s">
+        <v>80</v>
+      </c>
+      <c r="I5" t="s">
+        <v>87</v>
+      </c>
+      <c r="J5">
+        <v>4</v>
+      </c>
+      <c r="K5" s="1">
+        <v>5.8000000000000003E-2</v>
+      </c>
+      <c r="L5" s="1">
+        <f t="shared" ref="L5:L9" si="0">K5*J5</f>
+        <v>0.23200000000000001</v>
+      </c>
+      <c r="N5" s="5" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B6" t="s">
+        <v>69</v>
+      </c>
+      <c r="C6" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="E6" t="s">
+        <v>81</v>
+      </c>
+      <c r="I6" t="s">
+        <v>88</v>
+      </c>
+      <c r="J6">
+        <v>8</v>
+      </c>
+      <c r="K6" s="1">
+        <v>5.8000000000000003E-2</v>
+      </c>
+      <c r="L6" s="1">
+        <f t="shared" si="0"/>
+        <v>0.46400000000000002</v>
+      </c>
+      <c r="N6" s="5" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B7" t="s">
+        <v>82</v>
+      </c>
+      <c r="C7" s="1">
+        <f>L10</f>
+        <v>1.4880000000000004</v>
+      </c>
+      <c r="E7" t="s">
+        <v>94</v>
+      </c>
+      <c r="I7" t="s">
+        <v>91</v>
+      </c>
+      <c r="J7">
+        <v>4</v>
+      </c>
+      <c r="K7" s="1">
+        <v>2.5000000000000001E-2</v>
+      </c>
+      <c r="L7" s="1">
+        <f t="shared" si="0"/>
+        <v>0.1</v>
+      </c>
+      <c r="N7" s="5" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B8" t="s">
+        <v>48</v>
+      </c>
+      <c r="C8" s="1">
+        <v>1</v>
+      </c>
+      <c r="E8" t="s">
+        <v>81</v>
+      </c>
+      <c r="I8" t="s">
+        <v>89</v>
+      </c>
+      <c r="J8">
+        <v>4</v>
+      </c>
+      <c r="K8" s="1">
+        <v>3.3000000000000002E-2</v>
+      </c>
+      <c r="L8" s="1">
+        <f t="shared" si="0"/>
+        <v>0.13200000000000001</v>
+      </c>
+      <c r="N8" s="5" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>45</v>
+      </c>
+      <c r="C9" s="1">
+        <v>2</v>
+      </c>
+      <c r="E9" s="5"/>
+      <c r="I9" t="s">
+        <v>90</v>
+      </c>
+      <c r="J9">
+        <v>4</v>
+      </c>
+      <c r="K9" s="1">
+        <v>3.3000000000000002E-2</v>
+      </c>
+      <c r="L9" s="1">
+        <f t="shared" si="0"/>
+        <v>0.13200000000000001</v>
+      </c>
+      <c r="N9" s="5" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="C10" s="1"/>
+      <c r="K10" t="s">
+        <v>92</v>
+      </c>
+      <c r="L10" s="1">
+        <f>SUM(L4:L9)</f>
+        <v>1.4880000000000004</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A11" s="11" t="s">
+        <v>50</v>
+      </c>
+      <c r="B11" s="11"/>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B12" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.45">
-      <c r="A4" s="10" t="s">
-        <v>46</v>
-      </c>
-      <c r="B4" s="10"/>
-    </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.45">
-      <c r="B5" t="s">
-        <v>48</v>
-      </c>
-      <c r="C5" s="1">
-        <v>3.1</v>
-      </c>
-      <c r="E5" t="s">
+      <c r="C12" s="1">
+        <f>SUM(C3:C9)</f>
+        <v>11.384</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B13" t="s">
+        <v>51</v>
+      </c>
+      <c r="C13" s="1">
+        <v>34.99</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B14" t="s">
+        <v>54</v>
+      </c>
+      <c r="C14" s="7">
+        <f>C13-C12</f>
+        <v>23.606000000000002</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B15" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.45">
-      <c r="B6" t="s">
-        <v>54</v>
-      </c>
-      <c r="C6" s="1">
-        <v>0</v>
-      </c>
-      <c r="E6" t="s">
+      <c r="C15" s="6">
+        <f>C14/C12</f>
+        <v>2.0736120871398454</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B16" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.45">
-      <c r="B7" t="s">
-        <v>49</v>
-      </c>
-      <c r="C7" s="1">
-        <v>0.8</v>
-      </c>
-      <c r="E7" t="s">
+      <c r="C16" s="1">
+        <v>8.3000000000000007</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A18" s="4" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.45">
-      <c r="A8" t="s">
-        <v>50</v>
-      </c>
-      <c r="C8" s="1">
-        <v>2</v>
-      </c>
-      <c r="E8" s="5" t="s">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B19" t="s">
         <v>57</v>
       </c>
-      <c r="I8" s="4" t="s">
+      <c r="C19" s="1">
+        <v>15.29</v>
+      </c>
+      <c r="E19" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B20" t="s">
         <v>58</v>
       </c>
-      <c r="L8" t="s">
-        <v>95</v>
-      </c>
-      <c r="M8" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.45">
-      <c r="C9" s="1"/>
-      <c r="M9" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.45">
-      <c r="A10" s="11" t="s">
+      <c r="C20" s="1">
+        <v>38.950000000000003</v>
+      </c>
+      <c r="E20" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B21" t="s">
+        <v>59</v>
+      </c>
+      <c r="C21" s="1">
+        <v>9</v>
+      </c>
+      <c r="E21" s="5" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B22" t="s">
         <v>60</v>
       </c>
-      <c r="B10" s="11"/>
-    </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.45">
-      <c r="B11" t="s">
-        <v>62</v>
-      </c>
-      <c r="C11" s="1">
-        <f>SUM(C3:C8)</f>
-        <v>11.795999999999999</v>
-      </c>
-    </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.45">
-      <c r="B12" t="s">
-        <v>61</v>
-      </c>
-      <c r="C12" s="1">
-        <v>34.99</v>
-      </c>
-    </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.45">
-      <c r="B13" t="s">
+      <c r="C22" s="1">
+        <v>20</v>
+      </c>
+      <c r="E22" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B24" t="s">
         <v>64</v>
       </c>
-      <c r="C13" s="7">
-        <f>C12-C11</f>
-        <v>23.194000000000003</v>
-      </c>
-    </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.45">
-      <c r="B14" t="s">
-        <v>63</v>
-      </c>
-      <c r="C14" s="6">
-        <f>C13/C11</f>
-        <v>1.9662597490674809</v>
-      </c>
-    </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.45">
-      <c r="B15" t="s">
-        <v>65</v>
-      </c>
-      <c r="C15" s="1">
-        <v>8.3000000000000007</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A17" s="4" t="s">
+      <c r="C24" s="2">
+        <f>SUM(C19:C22)</f>
+        <v>83.240000000000009</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A26" s="4" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B27" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="B18" t="s">
-        <v>67</v>
-      </c>
-      <c r="C18" s="1">
-        <v>15.29</v>
-      </c>
-      <c r="E18" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="B19" t="s">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B28" s="4" t="s">
         <v>68</v>
       </c>
-      <c r="C19" s="1">
-        <v>38.950000000000003</v>
-      </c>
-      <c r="E19" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="B20" t="s">
-        <v>69</v>
-      </c>
-      <c r="C20" s="1">
-        <v>9</v>
-      </c>
-      <c r="E20" s="5" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="B21" t="s">
-        <v>70</v>
-      </c>
-      <c r="C21" s="1">
-        <v>20</v>
-      </c>
-      <c r="E21" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="B23" t="s">
-        <v>74</v>
-      </c>
-      <c r="C23" s="2">
-        <f>SUM(C18:C21)</f>
-        <v>83.240000000000009</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A25" s="4" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="B26" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="B27" s="4" t="s">
-        <v>78</v>
-      </c>
-      <c r="C27" s="2">
-        <f>C23+C15+C12</f>
+      <c r="C28" s="2">
+        <f>C24+C16+C13</f>
         <v>126.53</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="C28" s="2"/>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C29" s="2"/>
     </row>
   </sheetData>
   <mergeCells count="4">
     <mergeCell ref="A4:B4"/>
     <mergeCell ref="A1:C1"/>
     <mergeCell ref="A2:B2"/>
-    <mergeCell ref="A10:B10"/>
+    <mergeCell ref="A11:B11"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="E8" r:id="rId1" xr:uid="{00000000-0004-0000-0100-000000000000}"/>
-    <hyperlink ref="E20" r:id="rId2" xr:uid="{00000000-0004-0000-0100-000001000000}"/>
+    <hyperlink ref="E21" r:id="rId1" xr:uid="{00000000-0004-0000-0100-000001000000}"/>
+    <hyperlink ref="N4" r:id="rId2" xr:uid="{80CB4DE9-9BCD-4BFE-997C-8F2B1DA5DD84}"/>
+    <hyperlink ref="N7" r:id="rId3" xr:uid="{746C9000-2787-47A8-8F6A-7F1F08FBFF7C}"/>
+    <hyperlink ref="N5" r:id="rId4" xr:uid="{7AB6F59E-6AED-43CE-9DE5-F12A3ABAE69B}"/>
+    <hyperlink ref="N6" r:id="rId5" xr:uid="{9C44EF1F-64FF-4BDE-8C6E-75F41F8BD013}"/>
+    <hyperlink ref="N8" r:id="rId6" xr:uid="{9743D30C-D0CF-45E3-B56A-011BB141D88B}"/>
+    <hyperlink ref="N9" r:id="rId7" xr:uid="{F8039B6D-D15A-4507-B2DA-1674B068E10C}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId8"/>
 </worksheet>
 </file>
 
@@ -1706,21 +1974,21 @@
   <dimension ref="A1:I17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="29.73046875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="29.7109375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="22" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.73046875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="27.265625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="27.28515625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="14" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="19.59765625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="12.1328125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="19.5703125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1731,27 +1999,27 @@
         <v>2</v>
       </c>
       <c r="D1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E1" t="s">
+        <v>19</v>
+      </c>
+      <c r="F1" t="s">
         <v>15</v>
       </c>
-      <c r="E1" t="s">
-        <v>20</v>
-      </c>
-      <c r="F1" t="s">
-        <v>16</v>
-      </c>
       <c r="G1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="I1" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.45">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>6</v>
       </c>
       <c r="B2" t="s">
-        <v>91</v>
+        <v>78</v>
       </c>
       <c r="C2" t="s">
         <v>3</v>
@@ -1768,18 +2036,18 @@
         <v>5.16</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="I2" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.45">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>89</v>
+        <v>76</v>
       </c>
       <c r="C3" t="s">
         <v>4</v>
@@ -1795,17 +2063,19 @@
         <f t="shared" si="1"/>
         <v>7.0000000000000007E-2</v>
       </c>
-      <c r="G3" s="3"/>
+      <c r="G3" s="3" t="s">
+        <v>98</v>
+      </c>
       <c r="I3" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.45">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>1</v>
       </c>
       <c r="B4" t="s">
-        <v>90</v>
+        <v>77</v>
       </c>
       <c r="C4" t="s">
         <v>5</v>
@@ -1821,12 +2091,14 @@
         <f t="shared" si="1"/>
         <v>7.0000000000000007E-2</v>
       </c>
-      <c r="G4" s="3"/>
+      <c r="G4" s="3" t="s">
+        <v>98</v>
+      </c>
       <c r="I4" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.45">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>1</v>
       </c>
@@ -1834,27 +2106,27 @@
         <v>6</v>
       </c>
       <c r="C5" t="s">
-        <v>88</v>
+        <v>75</v>
       </c>
       <c r="D5">
         <f t="shared" si="0"/>
         <v>1000</v>
       </c>
       <c r="E5" s="1">
-        <v>1.85</v>
+        <v>0.2</v>
       </c>
       <c r="F5" s="1">
         <f t="shared" si="1"/>
-        <v>1.85</v>
-      </c>
-      <c r="G5" s="3" t="s">
-        <v>29</v>
+        <v>0.2</v>
+      </c>
+      <c r="G5" s="13" t="s">
+        <v>101</v>
       </c>
       <c r="I5" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.45">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>1</v>
       </c>
@@ -1862,33 +2134,33 @@
         <v>7</v>
       </c>
       <c r="C6" t="s">
-        <v>8</v>
+        <v>99</v>
       </c>
       <c r="D6">
         <f t="shared" si="0"/>
         <v>1000</v>
       </c>
       <c r="E6" s="1">
-        <v>0.18</v>
+        <v>0.17</v>
       </c>
       <c r="F6" s="1">
         <f t="shared" si="1"/>
-        <v>0.18</v>
+        <v>0.17</v>
       </c>
       <c r="G6" s="3"/>
-      <c r="I6" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="I6" s="12" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>2</v>
       </c>
       <c r="B7" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="C7" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D7">
         <f t="shared" si="0"/>
@@ -1903,18 +2175,18 @@
       </c>
       <c r="G7" s="3"/>
       <c r="I7" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.45">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>2</v>
       </c>
       <c r="B8" t="s">
-        <v>92</v>
+        <v>79</v>
       </c>
       <c r="C8" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D8">
         <f t="shared" si="0"/>
@@ -1929,18 +2201,18 @@
       </c>
       <c r="G8" s="3"/>
       <c r="I8" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.45">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>4</v>
       </c>
       <c r="B9" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C9" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D9">
         <f t="shared" si="0"/>
@@ -1955,27 +2227,27 @@
       </c>
       <c r="G9" s="3"/>
       <c r="I9" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.45">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="E10" s="1"/>
       <c r="F10" s="1"/>
       <c r="G10" s="3"/>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="E11" s="1" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="F11" s="1"/>
       <c r="G11" s="3"/>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>1</v>
       </c>
       <c r="B12" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D12">
         <f t="shared" si="0"/>
@@ -1989,15 +2261,15 @@
         <v>0.5</v>
       </c>
       <c r="G12" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.45">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>1</v>
       </c>
       <c r="B13" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D13">
         <f t="shared" si="0"/>
@@ -2011,15 +2283,15 @@
         <v>0.46</v>
       </c>
       <c r="G13" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.45">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>1</v>
       </c>
       <c r="B14" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="D14">
         <v>1000</v>
@@ -2032,33 +2304,37 @@
         <v>0.21</v>
       </c>
       <c r="G14" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.45">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="G15" s="3"/>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="E16" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="F16" s="1">
         <f>SUM(F2:F14)</f>
-        <v>8.5400000000000009</v>
+        <v>6.88</v>
       </c>
       <c r="I16" s="2"/>
     </row>
-    <row r="17" spans="5:6" x14ac:dyDescent="0.45">
+    <row r="17" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E17" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="F17" s="2">
         <f>F16*1.1</f>
-        <v>9.3940000000000019</v>
+        <v>7.5680000000000005</v>
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="I6" r:id="rId1" xr:uid="{83FC4712-112D-4C88-9AC5-9B7C88DB1F20}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -2067,20 +2343,20 @@
   <dimension ref="A1:I16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="J13" sqref="J13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="29.73046875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.3984375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.73046875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="27.265625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="29.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="27.28515625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="14" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="17.3984375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="17.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2091,27 +2367,27 @@
         <v>2</v>
       </c>
       <c r="D1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E1" t="s">
+        <v>19</v>
+      </c>
+      <c r="F1" t="s">
         <v>15</v>
       </c>
-      <c r="E1" t="s">
-        <v>20</v>
-      </c>
-      <c r="F1" t="s">
-        <v>16</v>
-      </c>
       <c r="G1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="I1" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.45">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>5</v>
       </c>
       <c r="B2" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="C2" t="s">
         <v>3</v>
@@ -2128,18 +2404,18 @@
         <v>4.3</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="I2" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.45">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C3" t="s">
         <v>4</v>
@@ -2155,17 +2431,19 @@
         <f t="shared" si="1"/>
         <v>7.0000000000000007E-2</v>
       </c>
-      <c r="G3" s="3"/>
+      <c r="G3" s="3" t="s">
+        <v>98</v>
+      </c>
       <c r="I3" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.45">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>1</v>
       </c>
       <c r="B4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C4" t="s">
         <v>5</v>
@@ -2181,12 +2459,14 @@
         <f t="shared" si="1"/>
         <v>7.0000000000000007E-2</v>
       </c>
-      <c r="G4" s="3"/>
+      <c r="G4" s="3" t="s">
+        <v>98</v>
+      </c>
       <c r="I4" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.45">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>1</v>
       </c>
@@ -2194,7 +2474,7 @@
         <v>7</v>
       </c>
       <c r="C5" t="s">
-        <v>8</v>
+        <v>99</v>
       </c>
       <c r="D5">
         <f t="shared" si="0"/>
@@ -2209,18 +2489,18 @@
       </c>
       <c r="G5" s="3"/>
       <c r="I5" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.45">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>2</v>
       </c>
       <c r="B6" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="C6" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D6">
         <f t="shared" si="0"/>
@@ -2235,18 +2515,18 @@
       </c>
       <c r="G6" s="3"/>
       <c r="I6" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.45">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>2</v>
       </c>
       <c r="B7" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="C7" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D7">
         <f t="shared" si="0"/>
@@ -2261,18 +2541,18 @@
       </c>
       <c r="G7" s="3"/>
       <c r="I7" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.45">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>2</v>
       </c>
       <c r="B8" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="C8" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D8">
         <f t="shared" si="0"/>
@@ -2287,18 +2567,18 @@
       </c>
       <c r="G8" s="3"/>
       <c r="I8" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.45">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>2</v>
       </c>
       <c r="B9" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="C9" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="D9">
         <f t="shared" ref="D9" si="2">1000*A9</f>
@@ -2313,22 +2593,22 @@
       </c>
       <c r="G9" s="3"/>
       <c r="I9" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.45">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="E10" s="1" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="F10" s="1"/>
       <c r="G10" s="3"/>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>1</v>
       </c>
       <c r="B11" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D11">
         <f t="shared" si="0"/>
@@ -2342,15 +2622,15 @@
         <v>0.3</v>
       </c>
       <c r="G11" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.45">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>1</v>
       </c>
       <c r="B12" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D12">
         <f t="shared" si="0"/>
@@ -2364,15 +2644,15 @@
         <v>0.26</v>
       </c>
       <c r="G12" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.45">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>1</v>
       </c>
       <c r="B13" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="D13">
         <v>1000</v>
@@ -2385,24 +2665,24 @@
         <v>0.14000000000000001</v>
       </c>
       <c r="G13" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.45">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="G14" s="3"/>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="E15" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="F15" s="1">
         <f>SUM(F2:F13)</f>
         <v>5.3599999999999985</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="E16" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="F16" s="2">
         <f>F15*1.1</f>

</xml_diff>

<commit_message>
Added Assembly Instructions and updated pricing
</commit_message>
<xml_diff>
--- a/Hardware/Estimated Financials.xlsx
+++ b/Hardware/Estimated Financials.xlsx
@@ -1,22 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21601"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Josh Johnson\Dropbox\ENGN4221\VeinCam2019\Hardware\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{422B842E-C8B3-47B2-B46F-F64FA45D2A8D}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B3921F40-C9E7-4667-9D1E-5BB539E705CF}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="28110" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="RPi 3A+ Total BOM" sheetId="4" r:id="rId1"/>
-    <sheet name="RPi Zero Total BOM" sheetId="3" r:id="rId2"/>
-    <sheet name="VeinCamHat BOM" sheetId="1" r:id="rId3"/>
-    <sheet name="VeinCamHatZero BOM" sheetId="2" r:id="rId4"/>
+    <sheet name="VeinCam BOM" sheetId="4" r:id="rId1"/>
+    <sheet name="VeinCamHat BOM" sheetId="1" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -31,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="194" uniqueCount="103">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="87">
   <si>
     <t>Qty</t>
   </si>
@@ -66,12 +64,6 @@
     <t>1k</t>
   </si>
   <si>
-    <t>D7, D9, D11</t>
-  </si>
-  <si>
-    <t>D8, D10, D12</t>
-  </si>
-  <si>
     <t>R3, R4, R5, R6</t>
   </si>
   <si>
@@ -96,9 +88,6 @@
     <t>Total Per Board (ex):</t>
   </si>
   <si>
-    <t>Total Per Board (inc):</t>
-  </si>
-  <si>
     <t>Notes</t>
   </si>
   <si>
@@ -132,27 +121,9 @@
     <t>PCBWAY Estimate</t>
   </si>
   <si>
-    <t>D1, D2, D3, D4, D6</t>
-  </si>
-  <si>
-    <t>R3, R4</t>
-  </si>
-  <si>
-    <t>R5, R8</t>
-  </si>
-  <si>
-    <t>R6, R7</t>
-  </si>
-  <si>
     <t>R1, R2</t>
   </si>
   <si>
-    <t>27R</t>
-  </si>
-  <si>
-    <t>https://www.digikey.com.au/product-detail/en/stackpole-electronics-inc/RMCF0603JT27R0/RMCF0603JT27R0CT-ND/2418191</t>
-  </si>
-  <si>
     <t>Total Cost at Quantity</t>
   </si>
   <si>
@@ -168,30 +139,15 @@
     <t>Per Unit Cost (Quantity 1000)</t>
   </si>
   <si>
-    <t>IR Filter</t>
-  </si>
-  <si>
     <t>Supplier</t>
   </si>
   <si>
-    <t>See VeinCamHatZero Sheet</t>
-  </si>
-  <si>
-    <t>Camera FFC</t>
-  </si>
-  <si>
-    <t>Bare Bones RPi Zero w/ offical case</t>
-  </si>
-  <si>
     <t>Estimated Total</t>
   </si>
   <si>
     <t>Sale Price</t>
   </si>
   <si>
-    <t>Cost Price (inc)</t>
-  </si>
-  <si>
     <t>Markup</t>
   </si>
   <si>
@@ -204,9 +160,6 @@
     <t>Customer Supplied Items:</t>
   </si>
   <si>
-    <t>Raspberry Pi Zero W</t>
-  </si>
-  <si>
     <t>PinoIR Camera Module</t>
   </si>
   <si>
@@ -219,18 +172,12 @@
     <t>https://core-electronics.com.au/raspberry-pi-noir-camera-board-v2-8-megapixels-38553.html</t>
   </si>
   <si>
-    <t>https://core-electronics.com.au/raspberry-pi-zero-w-wireless.html</t>
-  </si>
-  <si>
     <t>https://www.officeworks.com.au/shop/officeworks/p/sandisk-ultra-16gb-micro-sdhc-memory-card-sdsq16gb</t>
   </si>
   <si>
     <t>Cost of Customer Items</t>
   </si>
   <si>
-    <t>Ebay / may already own required parts</t>
-  </si>
-  <si>
     <t>Excludes freight on self supplied items</t>
   </si>
   <si>
@@ -240,12 +187,6 @@
     <t>Total</t>
   </si>
   <si>
-    <t>Labour to cut acrylic</t>
-  </si>
-  <si>
-    <t>Acrylic</t>
-  </si>
-  <si>
     <t>Mounting hardware</t>
   </si>
   <si>
@@ -273,12 +214,6 @@
     <t>R7, R8</t>
   </si>
   <si>
-    <t>Generic Item - 3mm Acrylic</t>
-  </si>
-  <si>
-    <t>TBD</t>
-  </si>
-  <si>
     <t>Mounting Hardware</t>
   </si>
   <si>
@@ -327,19 +262,34 @@
     <t>https://www.aliexpress.com/item/50Pcs-DIN934-M2-M2-5-M3-M4-M5-M6-M8-304-Stainless-Steel-Metric-Thread-Hex/32958861614.html?spm=a2g0s.9042311.0.0.1f924c4dMJUkZe</t>
   </si>
   <si>
-    <t>$0.02 from China</t>
-  </si>
-  <si>
     <t>NTJD4001N</t>
   </si>
   <si>
     <t>https://www.digikey.com.au/product-detail/en/on-semiconductor/NTJD4001NT1G/NTJD4001NT1GOSCT-ND/687105</t>
   </si>
   <si>
-    <t>China Price' shown</t>
-  </si>
-  <si>
-    <t>Ebay / may already own</t>
+    <t>IR Filter Acrylic</t>
+  </si>
+  <si>
+    <t>Clear Acrylic + Labour</t>
+  </si>
+  <si>
+    <t>RPi 3A+, VeinCam, Clear Acrylic Case</t>
+  </si>
+  <si>
+    <t>https://www.ebay.com.au/itm/50000mAh-External-Power-Bank-Dual-USB-Portable-Battery-Charger-For-Mobile-Phone/391554571425?hash=item5b2a789ca1:m:mPDj03kABY57qV9q2LbqCMQ</t>
+  </si>
+  <si>
+    <t>Cost Price (inc GST)</t>
+  </si>
+  <si>
+    <t>China Price shown</t>
+  </si>
+  <si>
+    <t>Cost Price (ex GST)</t>
+  </si>
+  <si>
+    <t>Assuming $150 for 50*50mm</t>
   </si>
 </sst>
 </file>
@@ -843,18 +793,23 @@
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="44"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="2" applyFont="1"/>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="44" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="1" quotePrefix="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -864,8 +819,9 @@
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="44" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="1" quotePrefix="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="45">
     <cellStyle name="20% - Accent1" xfId="21" builtinId="30" customBuiltin="1"/>
@@ -1224,269 +1180,269 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:O27"/>
+  <dimension ref="A1:N27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E22" sqref="E22"/>
+      <selection sqref="A1:C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="22.140625" customWidth="1"/>
     <col min="3" max="3" width="14.42578125" customWidth="1"/>
-    <col min="10" max="10" width="18.85546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="18.85546875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="8.7109375" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="10.28515625" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="9.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A1" s="9" t="s">
-        <v>49</v>
-      </c>
-      <c r="B1" s="9"/>
-      <c r="C1" s="9"/>
-    </row>
-    <row r="2" spans="1:15" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="9" t="s">
-        <v>41</v>
-      </c>
-      <c r="B2" s="9"/>
-      <c r="C2" s="8" t="s">
-        <v>44</v>
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A1" s="12" t="s">
+        <v>81</v>
+      </c>
+      <c r="B1" s="12"/>
+      <c r="C1" s="12"/>
+    </row>
+    <row r="2" spans="1:14" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="12" t="s">
+        <v>32</v>
+      </c>
+      <c r="B2" s="12"/>
+      <c r="C2" s="7" t="s">
+        <v>35</v>
       </c>
       <c r="D2" s="4"/>
       <c r="E2" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>42</v>
+        <v>33</v>
       </c>
       <c r="C3" s="2">
-        <f>'VeinCamHat BOM'!F17</f>
-        <v>7.5680000000000005</v>
+        <f>'VeinCamHat BOM'!F16</f>
+        <v>6.7799999999999985</v>
       </c>
       <c r="E3" t="s">
-        <v>74</v>
+        <v>55</v>
+      </c>
+      <c r="I3" t="s">
+        <v>61</v>
       </c>
       <c r="J3" t="s">
-        <v>82</v>
+        <v>62</v>
       </c>
       <c r="K3" t="s">
-        <v>83</v>
+        <v>63</v>
       </c>
       <c r="L3" t="s">
-        <v>84</v>
-      </c>
-      <c r="M3" t="s">
-        <v>85</v>
-      </c>
-      <c r="O3" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A4" s="10" t="s">
-        <v>43</v>
-      </c>
-      <c r="B4" s="10"/>
-      <c r="J4" t="s">
+        <v>64</v>
+      </c>
+      <c r="N3" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A4" s="13" t="s">
+        <v>34</v>
+      </c>
+      <c r="B4" s="13"/>
+      <c r="I4" t="s">
+        <v>65</v>
+      </c>
+      <c r="J4">
+        <v>4</v>
+      </c>
+      <c r="K4" s="1">
+        <v>0.107</v>
+      </c>
+      <c r="L4" s="1">
+        <f>K4*J4</f>
+        <v>0.42799999999999999</v>
+      </c>
+      <c r="N4" s="11" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B5" t="s">
+        <v>80</v>
+      </c>
+      <c r="C5" s="1">
+        <v>2.5</v>
+      </c>
+      <c r="I5" t="s">
+        <v>66</v>
+      </c>
+      <c r="J5">
+        <v>4</v>
+      </c>
+      <c r="K5" s="1">
+        <v>5.8000000000000003E-2</v>
+      </c>
+      <c r="L5" s="1">
+        <f t="shared" ref="L5:L9" si="0">K5*J5</f>
+        <v>0.23200000000000001</v>
+      </c>
+      <c r="N5" s="11" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B6" t="s">
+        <v>79</v>
+      </c>
+      <c r="C6" s="1">
+        <v>1.5</v>
+      </c>
+      <c r="E6" t="s">
         <v>86</v>
       </c>
-      <c r="K4">
-        <v>4</v>
-      </c>
-      <c r="L4" s="1">
-        <v>0.107</v>
-      </c>
-      <c r="M4" s="1">
-        <f>L4*K4</f>
-        <v>0.42799999999999999</v>
-      </c>
-      <c r="O4" s="5" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="B5" t="s">
-        <v>70</v>
-      </c>
-      <c r="C5" s="1">
-        <v>0.5</v>
-      </c>
-      <c r="E5" t="s">
-        <v>80</v>
-      </c>
-      <c r="J5" t="s">
-        <v>87</v>
-      </c>
-      <c r="K5">
-        <v>4</v>
-      </c>
-      <c r="L5" s="1">
+      <c r="I6" t="s">
+        <v>67</v>
+      </c>
+      <c r="J6">
+        <v>8</v>
+      </c>
+      <c r="K6" s="1">
         <v>5.8000000000000003E-2</v>
       </c>
-      <c r="M5" s="1">
-        <f t="shared" ref="M5:M9" si="0">L5*K5</f>
-        <v>0.23200000000000001</v>
-      </c>
-      <c r="O5" s="5" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="B6" t="s">
-        <v>69</v>
-      </c>
-      <c r="C6" s="1">
-        <v>0.5</v>
-      </c>
-      <c r="E6" t="s">
-        <v>81</v>
-      </c>
-      <c r="J6" t="s">
-        <v>88</v>
-      </c>
-      <c r="K6">
-        <v>8</v>
-      </c>
       <c r="L6" s="1">
-        <v>5.8000000000000003E-2</v>
-      </c>
-      <c r="M6" s="1">
         <f t="shared" si="0"/>
         <v>0.46400000000000002</v>
       </c>
-      <c r="O6" s="5" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="N6" s="11" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
-        <v>71</v>
+        <v>52</v>
       </c>
       <c r="C7" s="1">
-        <f>M10</f>
+        <f>L11</f>
         <v>1.4880000000000004</v>
       </c>
       <c r="E7" t="s">
-        <v>94</v>
-      </c>
-      <c r="J7" t="s">
-        <v>91</v>
-      </c>
-      <c r="K7">
+        <v>73</v>
+      </c>
+      <c r="I7" t="s">
+        <v>70</v>
+      </c>
+      <c r="J7">
         <v>4</v>
       </c>
+      <c r="K7" s="1">
+        <v>2.5000000000000001E-2</v>
+      </c>
       <c r="L7" s="1">
-        <v>2.5000000000000001E-2</v>
-      </c>
-      <c r="M7" s="1">
         <f t="shared" si="0"/>
         <v>0.1</v>
       </c>
-      <c r="O7" s="5" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>45</v>
-      </c>
-      <c r="C8" s="1">
-        <v>2</v>
-      </c>
-      <c r="E8" s="12" t="s">
-        <v>81</v>
-      </c>
-      <c r="J8" t="s">
-        <v>89</v>
-      </c>
-      <c r="K8">
+      <c r="N7" s="11" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="C8" s="1"/>
+      <c r="I8" t="s">
+        <v>68</v>
+      </c>
+      <c r="J8">
         <v>4</v>
       </c>
+      <c r="K8" s="1">
+        <v>3.3000000000000002E-2</v>
+      </c>
       <c r="L8" s="1">
-        <v>3.3000000000000002E-2</v>
-      </c>
-      <c r="M8" s="1">
         <f t="shared" si="0"/>
         <v>0.13200000000000001</v>
       </c>
-      <c r="O8" s="5" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="C9" s="1"/>
-      <c r="J9" t="s">
-        <v>90</v>
-      </c>
-      <c r="K9">
+      <c r="N8" s="11" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A9" s="14" t="s">
+        <v>37</v>
+      </c>
+      <c r="B9" s="14"/>
+      <c r="I9" t="s">
+        <v>69</v>
+      </c>
+      <c r="J9">
         <v>4</v>
       </c>
+      <c r="K9" s="1">
+        <v>3.3000000000000002E-2</v>
+      </c>
       <c r="L9" s="1">
-        <v>3.3000000000000002E-2</v>
-      </c>
-      <c r="M9" s="1">
         <f t="shared" si="0"/>
         <v>0.13200000000000001</v>
       </c>
-      <c r="O9" s="5" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A10" s="11" t="s">
-        <v>50</v>
-      </c>
-      <c r="B10" s="11"/>
-      <c r="L10" t="s">
-        <v>92</v>
-      </c>
-      <c r="M10" s="1">
-        <f>SUM(M4:M9)</f>
+      <c r="N9" s="11" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A10" s="10"/>
+      <c r="B10" s="15" t="s">
+        <v>85</v>
+      </c>
+      <c r="C10" s="2">
+        <f>SUM(C3:C7)</f>
+        <v>12.267999999999997</v>
+      </c>
+      <c r="K10" s="1"/>
+      <c r="L10" s="1"/>
+      <c r="N10" s="11"/>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B11" t="s">
+        <v>83</v>
+      </c>
+      <c r="C11" s="1">
+        <f>C10*1.1</f>
+        <v>13.494799999999998</v>
+      </c>
+      <c r="K11" t="s">
+        <v>71</v>
+      </c>
+      <c r="L11" s="1">
+        <f>SUM(L4:L9)</f>
         <v>1.4880000000000004</v>
       </c>
     </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="B11" t="s">
-        <v>52</v>
-      </c>
-      <c r="C11" s="1">
-        <f>SUM(C3:C8)</f>
-        <v>12.056000000000001</v>
-      </c>
-    </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
-        <v>51</v>
+        <v>38</v>
       </c>
       <c r="C12" s="1">
         <v>39.99</v>
       </c>
     </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
-        <v>54</v>
-      </c>
-      <c r="C13" s="7">
+        <v>40</v>
+      </c>
+      <c r="C13" s="6">
         <f>C12-C11</f>
-        <v>27.934000000000001</v>
-      </c>
-    </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
+        <v>26.495200000000004</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
-        <v>53</v>
-      </c>
-      <c r="C14" s="6">
+        <v>39</v>
+      </c>
+      <c r="C14" s="5">
         <f>C13/C11</f>
-        <v>2.3170205706702056</v>
-      </c>
-    </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
+        <v>1.9633636660046838</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
-        <v>55</v>
+        <v>41</v>
       </c>
       <c r="C15" s="1">
         <v>8.3000000000000007</v>
@@ -1494,79 +1450,79 @@
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="4" t="s">
-        <v>56</v>
+        <v>42</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B18" t="s">
-        <v>72</v>
+        <v>53</v>
       </c>
       <c r="C18" s="1">
         <v>38.229999999999997</v>
       </c>
       <c r="E18" t="s">
-        <v>73</v>
+        <v>54</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B19" t="s">
-        <v>58</v>
+        <v>43</v>
       </c>
       <c r="C19" s="1">
         <v>38.950000000000003</v>
       </c>
       <c r="E19" t="s">
-        <v>61</v>
+        <v>46</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B20" t="s">
-        <v>59</v>
+        <v>44</v>
       </c>
       <c r="C20" s="1">
         <v>9</v>
       </c>
-      <c r="E20" s="5" t="s">
-        <v>63</v>
+      <c r="E20" s="11" t="s">
+        <v>47</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B21" t="s">
-        <v>60</v>
+        <v>45</v>
       </c>
       <c r="C21" s="1">
-        <v>20</v>
-      </c>
-      <c r="E21" t="s">
-        <v>102</v>
+        <v>12.95</v>
+      </c>
+      <c r="E21" s="11" t="s">
+        <v>82</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B23" t="s">
-        <v>64</v>
+        <v>48</v>
       </c>
       <c r="C23" s="2">
         <f>SUM(C18:C21)</f>
-        <v>106.18</v>
+        <v>99.13000000000001</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" s="4" t="s">
-        <v>67</v>
+        <v>50</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B26" t="s">
-        <v>66</v>
+        <v>49</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B27" s="4" t="s">
-        <v>68</v>
+        <v>51</v>
       </c>
       <c r="C27" s="2">
         <f>C23+C15+C12</f>
-        <v>154.47</v>
+        <v>147.42000000000002</v>
       </c>
     </row>
   </sheetData>
@@ -1574,407 +1530,19 @@
     <mergeCell ref="A1:C1"/>
     <mergeCell ref="A2:B2"/>
     <mergeCell ref="A4:B4"/>
-    <mergeCell ref="A10:B10"/>
+    <mergeCell ref="A9:B9"/>
   </mergeCells>
-  <hyperlinks>
-    <hyperlink ref="E20" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
-    <hyperlink ref="O4" r:id="rId2" xr:uid="{15831DEE-A6A1-4D03-BA9B-B20F6C6807D4}"/>
-    <hyperlink ref="O7" r:id="rId3" xr:uid="{9B98D2E0-877B-4C9B-8F40-18E6E7ADCCEE}"/>
-    <hyperlink ref="O5" r:id="rId4" xr:uid="{CA668A5A-75C5-4964-9717-E58376AF80AA}"/>
-    <hyperlink ref="O6" r:id="rId5" xr:uid="{0FA79612-40E9-44C6-A6A1-0DCBDF1B8A6B}"/>
-    <hyperlink ref="O8" r:id="rId6" xr:uid="{B27C6BF6-FA47-4A12-8E8E-E3982DFB9EEB}"/>
-    <hyperlink ref="O9" r:id="rId7" xr:uid="{5E636539-9201-4464-A8E8-CA351037BED5}"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:N29"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F38" sqref="F38"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="9.85546875" customWidth="1"/>
-    <col min="2" max="2" width="22" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="5.42578125" customWidth="1"/>
-    <col min="12" max="12" width="10.5703125" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A1" s="9" t="s">
-        <v>49</v>
-      </c>
-      <c r="B1" s="9"/>
-      <c r="C1" s="9"/>
-    </row>
-    <row r="2" spans="1:14" ht="30" x14ac:dyDescent="0.25">
-      <c r="A2" s="9" t="s">
-        <v>41</v>
-      </c>
-      <c r="B2" s="9"/>
-      <c r="C2" s="8" t="s">
-        <v>44</v>
-      </c>
-      <c r="D2" s="4"/>
-      <c r="E2" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>42</v>
-      </c>
-      <c r="C3" s="2">
-        <f>'VeinCamHatZero BOM'!F16</f>
-        <v>5.895999999999999</v>
-      </c>
-      <c r="E3" t="s">
-        <v>47</v>
-      </c>
-      <c r="I3" t="s">
-        <v>82</v>
-      </c>
-      <c r="J3" t="s">
-        <v>83</v>
-      </c>
-      <c r="K3" t="s">
-        <v>84</v>
-      </c>
-      <c r="L3" t="s">
-        <v>85</v>
-      </c>
-      <c r="N3" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A4" s="10" t="s">
-        <v>43</v>
-      </c>
-      <c r="B4" s="10"/>
-      <c r="I4" t="s">
-        <v>86</v>
-      </c>
-      <c r="J4">
-        <v>4</v>
-      </c>
-      <c r="K4" s="1">
-        <v>0.107</v>
-      </c>
-      <c r="L4" s="1">
-        <f>K4*J4</f>
-        <v>0.42799999999999999</v>
-      </c>
-      <c r="N4" s="5" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="B5" t="s">
-        <v>70</v>
-      </c>
-      <c r="C5" s="1">
-        <v>0.5</v>
-      </c>
-      <c r="E5" t="s">
-        <v>80</v>
-      </c>
-      <c r="I5" t="s">
-        <v>87</v>
-      </c>
-      <c r="J5">
-        <v>4</v>
-      </c>
-      <c r="K5" s="1">
-        <v>5.8000000000000003E-2</v>
-      </c>
-      <c r="L5" s="1">
-        <f t="shared" ref="L5:L9" si="0">K5*J5</f>
-        <v>0.23200000000000001</v>
-      </c>
-      <c r="N5" s="5" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="B6" t="s">
-        <v>69</v>
-      </c>
-      <c r="C6" s="1">
-        <v>0.5</v>
-      </c>
-      <c r="E6" t="s">
-        <v>81</v>
-      </c>
-      <c r="I6" t="s">
-        <v>88</v>
-      </c>
-      <c r="J6">
-        <v>8</v>
-      </c>
-      <c r="K6" s="1">
-        <v>5.8000000000000003E-2</v>
-      </c>
-      <c r="L6" s="1">
-        <f t="shared" si="0"/>
-        <v>0.46400000000000002</v>
-      </c>
-      <c r="N6" s="5" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="B7" t="s">
-        <v>82</v>
-      </c>
-      <c r="C7" s="1">
-        <f>L10</f>
-        <v>1.4880000000000004</v>
-      </c>
-      <c r="E7" t="s">
-        <v>94</v>
-      </c>
-      <c r="I7" t="s">
-        <v>91</v>
-      </c>
-      <c r="J7">
-        <v>4</v>
-      </c>
-      <c r="K7" s="1">
-        <v>2.5000000000000001E-2</v>
-      </c>
-      <c r="L7" s="1">
-        <f t="shared" si="0"/>
-        <v>0.1</v>
-      </c>
-      <c r="N7" s="5" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="B8" t="s">
-        <v>48</v>
-      </c>
-      <c r="C8" s="1">
-        <v>1</v>
-      </c>
-      <c r="E8" t="s">
-        <v>81</v>
-      </c>
-      <c r="I8" t="s">
-        <v>89</v>
-      </c>
-      <c r="J8">
-        <v>4</v>
-      </c>
-      <c r="K8" s="1">
-        <v>3.3000000000000002E-2</v>
-      </c>
-      <c r="L8" s="1">
-        <f t="shared" si="0"/>
-        <v>0.13200000000000001</v>
-      </c>
-      <c r="N8" s="5" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>45</v>
-      </c>
-      <c r="C9" s="1">
-        <v>2</v>
-      </c>
-      <c r="E9" s="5"/>
-      <c r="I9" t="s">
-        <v>90</v>
-      </c>
-      <c r="J9">
-        <v>4</v>
-      </c>
-      <c r="K9" s="1">
-        <v>3.3000000000000002E-2</v>
-      </c>
-      <c r="L9" s="1">
-        <f t="shared" si="0"/>
-        <v>0.13200000000000001</v>
-      </c>
-      <c r="N9" s="5" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="C10" s="1"/>
-      <c r="K10" t="s">
-        <v>92</v>
-      </c>
-      <c r="L10" s="1">
-        <f>SUM(L4:L9)</f>
-        <v>1.4880000000000004</v>
-      </c>
-    </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A11" s="11" t="s">
-        <v>50</v>
-      </c>
-      <c r="B11" s="11"/>
-    </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="B12" t="s">
-        <v>52</v>
-      </c>
-      <c r="C12" s="1">
-        <f>SUM(C3:C9)</f>
-        <v>11.384</v>
-      </c>
-    </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="B13" t="s">
-        <v>51</v>
-      </c>
-      <c r="C13" s="1">
-        <v>34.99</v>
-      </c>
-    </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="B14" t="s">
-        <v>54</v>
-      </c>
-      <c r="C14" s="7">
-        <f>C13-C12</f>
-        <v>23.606000000000002</v>
-      </c>
-    </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="B15" t="s">
-        <v>53</v>
-      </c>
-      <c r="C15" s="6">
-        <f>C14/C12</f>
-        <v>2.0736120871398454</v>
-      </c>
-    </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="B16" t="s">
-        <v>55</v>
-      </c>
-      <c r="C16" s="1">
-        <v>8.3000000000000007</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A18" s="4" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B19" t="s">
-        <v>57</v>
-      </c>
-      <c r="C19" s="1">
-        <v>15.29</v>
-      </c>
-      <c r="E19" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B20" t="s">
-        <v>58</v>
-      </c>
-      <c r="C20" s="1">
-        <v>38.950000000000003</v>
-      </c>
-      <c r="E20" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B21" t="s">
-        <v>59</v>
-      </c>
-      <c r="C21" s="1">
-        <v>9</v>
-      </c>
-      <c r="E21" s="5" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B22" t="s">
-        <v>60</v>
-      </c>
-      <c r="C22" s="1">
-        <v>20</v>
-      </c>
-      <c r="E22" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B24" t="s">
-        <v>64</v>
-      </c>
-      <c r="C24" s="2">
-        <f>SUM(C19:C22)</f>
-        <v>83.240000000000009</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A26" s="4" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B27" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B28" s="4" t="s">
-        <v>68</v>
-      </c>
-      <c r="C28" s="2">
-        <f>C24+C16+C13</f>
-        <v>126.53</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="C29" s="2"/>
-    </row>
-  </sheetData>
-  <mergeCells count="4">
-    <mergeCell ref="A4:B4"/>
-    <mergeCell ref="A1:C1"/>
-    <mergeCell ref="A2:B2"/>
-    <mergeCell ref="A11:B11"/>
-  </mergeCells>
-  <hyperlinks>
-    <hyperlink ref="E21" r:id="rId1" xr:uid="{00000000-0004-0000-0100-000001000000}"/>
-    <hyperlink ref="N4" r:id="rId2" xr:uid="{80CB4DE9-9BCD-4BFE-997C-8F2B1DA5DD84}"/>
-    <hyperlink ref="N7" r:id="rId3" xr:uid="{746C9000-2787-47A8-8F6A-7F1F08FBFF7C}"/>
-    <hyperlink ref="N5" r:id="rId4" xr:uid="{7AB6F59E-6AED-43CE-9DE5-F12A3ABAE69B}"/>
-    <hyperlink ref="N6" r:id="rId5" xr:uid="{9C44EF1F-64FF-4BDE-8C6E-75F41F8BD013}"/>
-    <hyperlink ref="N8" r:id="rId6" xr:uid="{9743D30C-D0CF-45E3-B56A-011BB141D88B}"/>
-    <hyperlink ref="N9" r:id="rId7" xr:uid="{F8039B6D-D15A-4507-B2DA-1674B068E10C}"/>
-  </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId8"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:I17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+      <selection activeCell="E17" sqref="E17:F17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1999,19 +1567,19 @@
         <v>2</v>
       </c>
       <c r="D1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="E1" t="s">
+        <v>17</v>
+      </c>
+      <c r="F1" t="s">
+        <v>13</v>
+      </c>
+      <c r="G1" t="s">
         <v>19</v>
       </c>
-      <c r="F1" t="s">
-        <v>15</v>
-      </c>
-      <c r="G1" t="s">
-        <v>22</v>
-      </c>
       <c r="I1" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
@@ -2019,7 +1587,7 @@
         <v>6</v>
       </c>
       <c r="B2" t="s">
-        <v>78</v>
+        <v>59</v>
       </c>
       <c r="C2" t="s">
         <v>3</v>
@@ -2036,10 +1604,10 @@
         <v>5.16</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="I2" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
@@ -2047,7 +1615,7 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>76</v>
+        <v>57</v>
       </c>
       <c r="C3" t="s">
         <v>4</v>
@@ -2057,17 +1625,17 @@
         <v>1000</v>
       </c>
       <c r="E3" s="1">
-        <v>7.0000000000000007E-2</v>
+        <v>0.02</v>
       </c>
       <c r="F3" s="1">
         <f t="shared" si="1"/>
-        <v>7.0000000000000007E-2</v>
-      </c>
-      <c r="G3" s="3" t="s">
-        <v>98</v>
+        <v>0.02</v>
+      </c>
+      <c r="G3" s="9" t="s">
+        <v>84</v>
       </c>
       <c r="I3" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
@@ -2075,7 +1643,7 @@
         <v>1</v>
       </c>
       <c r="B4" t="s">
-        <v>77</v>
+        <v>58</v>
       </c>
       <c r="C4" t="s">
         <v>5</v>
@@ -2085,17 +1653,17 @@
         <v>1000</v>
       </c>
       <c r="E4" s="1">
-        <v>7.0000000000000007E-2</v>
+        <v>0.02</v>
       </c>
       <c r="F4" s="1">
         <f t="shared" si="1"/>
-        <v>7.0000000000000007E-2</v>
-      </c>
-      <c r="G4" s="3" t="s">
-        <v>98</v>
+        <v>0.02</v>
+      </c>
+      <c r="G4" s="9" t="s">
+        <v>84</v>
       </c>
       <c r="I4" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
@@ -2106,7 +1674,7 @@
         <v>6</v>
       </c>
       <c r="C5" t="s">
-        <v>75</v>
+        <v>56</v>
       </c>
       <c r="D5">
         <f t="shared" si="0"/>
@@ -2119,11 +1687,11 @@
         <f t="shared" si="1"/>
         <v>0.2</v>
       </c>
-      <c r="G5" s="13" t="s">
-        <v>101</v>
+      <c r="G5" s="9" t="s">
+        <v>84</v>
       </c>
       <c r="I5" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
@@ -2134,7 +1702,7 @@
         <v>7</v>
       </c>
       <c r="C6" t="s">
-        <v>99</v>
+        <v>77</v>
       </c>
       <c r="D6">
         <f t="shared" si="0"/>
@@ -2148,8 +1716,8 @@
         <v>0.17</v>
       </c>
       <c r="G6" s="3"/>
-      <c r="I6" s="12" t="s">
-        <v>100</v>
+      <c r="I6" s="8" t="s">
+        <v>78</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
@@ -2157,7 +1725,7 @@
         <v>2</v>
       </c>
       <c r="B7" t="s">
-        <v>37</v>
+        <v>30</v>
       </c>
       <c r="C7" t="s">
         <v>10</v>
@@ -2175,7 +1743,7 @@
       </c>
       <c r="G7" s="3"/>
       <c r="I7" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
@@ -2183,7 +1751,7 @@
         <v>2</v>
       </c>
       <c r="B8" t="s">
-        <v>79</v>
+        <v>60</v>
       </c>
       <c r="C8" t="s">
         <v>9</v>
@@ -2201,7 +1769,7 @@
       </c>
       <c r="G8" s="3"/>
       <c r="I8" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
@@ -2209,7 +1777,7 @@
         <v>4</v>
       </c>
       <c r="B9" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C9" t="s">
         <v>8</v>
@@ -2227,7 +1795,7 @@
       </c>
       <c r="G9" s="3"/>
       <c r="I9" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
@@ -2237,7 +1805,7 @@
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="E11" s="1" t="s">
-        <v>40</v>
+        <v>31</v>
       </c>
       <c r="F11" s="1"/>
       <c r="G11" s="3"/>
@@ -2247,7 +1815,7 @@
         <v>1</v>
       </c>
       <c r="B12" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="D12">
         <f t="shared" si="0"/>
@@ -2261,7 +1829,7 @@
         <v>0.5</v>
       </c>
       <c r="G12" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
@@ -2269,7 +1837,7 @@
         <v>1</v>
       </c>
       <c r="B13" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="D13">
         <f t="shared" si="0"/>
@@ -2283,7 +1851,7 @@
         <v>0.46</v>
       </c>
       <c r="G13" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
@@ -2291,7 +1859,7 @@
         <v>1</v>
       </c>
       <c r="B14" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="D14">
         <v>1000</v>
@@ -2304,7 +1872,7 @@
         <v>0.21</v>
       </c>
       <c r="G14" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
@@ -2312,22 +1880,16 @@
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="E16" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="F16" s="1">
         <f>SUM(F2:F14)</f>
-        <v>6.88</v>
+        <v>6.7799999999999985</v>
       </c>
       <c r="I16" s="2"/>
     </row>
-    <row r="17" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E17" t="s">
-        <v>21</v>
-      </c>
-      <c r="F17" s="2">
-        <f>F16*1.1</f>
-        <v>7.5680000000000005</v>
-      </c>
+    <row r="17" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F17" s="2"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -2336,360 +1898,4 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:I16"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J13" sqref="J13"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="2" max="2" width="29.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="27.28515625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="17.42578125" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" t="s">
-        <v>14</v>
-      </c>
-      <c r="E1" t="s">
-        <v>19</v>
-      </c>
-      <c r="F1" t="s">
-        <v>15</v>
-      </c>
-      <c r="G1" t="s">
-        <v>22</v>
-      </c>
-      <c r="I1" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A2">
-        <v>5</v>
-      </c>
-      <c r="B2" t="s">
-        <v>33</v>
-      </c>
-      <c r="C2" t="s">
-        <v>3</v>
-      </c>
-      <c r="D2">
-        <f t="shared" ref="D2:D12" si="0">1000*A2</f>
-        <v>5000</v>
-      </c>
-      <c r="E2" s="1">
-        <v>0.86</v>
-      </c>
-      <c r="F2" s="1">
-        <f t="shared" ref="F2:F8" si="1">E2*A2</f>
-        <v>4.3</v>
-      </c>
-      <c r="G2" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="I2" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A3">
-        <v>1</v>
-      </c>
-      <c r="B3" t="s">
-        <v>11</v>
-      </c>
-      <c r="C3" t="s">
-        <v>4</v>
-      </c>
-      <c r="D3">
-        <f t="shared" si="0"/>
-        <v>1000</v>
-      </c>
-      <c r="E3" s="1">
-        <v>7.0000000000000007E-2</v>
-      </c>
-      <c r="F3" s="1">
-        <f t="shared" si="1"/>
-        <v>7.0000000000000007E-2</v>
-      </c>
-      <c r="G3" s="3" t="s">
-        <v>98</v>
-      </c>
-      <c r="I3" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A4">
-        <v>1</v>
-      </c>
-      <c r="B4" t="s">
-        <v>12</v>
-      </c>
-      <c r="C4" t="s">
-        <v>5</v>
-      </c>
-      <c r="D4">
-        <f t="shared" si="0"/>
-        <v>1000</v>
-      </c>
-      <c r="E4" s="1">
-        <v>7.0000000000000007E-2</v>
-      </c>
-      <c r="F4" s="1">
-        <f t="shared" si="1"/>
-        <v>7.0000000000000007E-2</v>
-      </c>
-      <c r="G4" s="3" t="s">
-        <v>98</v>
-      </c>
-      <c r="I4" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A5">
-        <v>1</v>
-      </c>
-      <c r="B5" t="s">
-        <v>7</v>
-      </c>
-      <c r="C5" t="s">
-        <v>99</v>
-      </c>
-      <c r="D5">
-        <f t="shared" si="0"/>
-        <v>1000</v>
-      </c>
-      <c r="E5" s="1">
-        <v>0.18</v>
-      </c>
-      <c r="F5" s="1">
-        <f t="shared" si="1"/>
-        <v>0.18</v>
-      </c>
-      <c r="G5" s="3"/>
-      <c r="I5" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A6">
-        <v>2</v>
-      </c>
-      <c r="B6" t="s">
-        <v>34</v>
-      </c>
-      <c r="C6" t="s">
-        <v>8</v>
-      </c>
-      <c r="D6">
-        <f t="shared" si="0"/>
-        <v>2000</v>
-      </c>
-      <c r="E6" s="1">
-        <v>5.0000000000000001E-3</v>
-      </c>
-      <c r="F6" s="1">
-        <f t="shared" si="1"/>
-        <v>0.01</v>
-      </c>
-      <c r="G6" s="3"/>
-      <c r="I6" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A7">
-        <v>2</v>
-      </c>
-      <c r="B7" t="s">
-        <v>35</v>
-      </c>
-      <c r="C7" t="s">
-        <v>9</v>
-      </c>
-      <c r="D7">
-        <f t="shared" si="0"/>
-        <v>2000</v>
-      </c>
-      <c r="E7" s="1">
-        <v>5.0000000000000001E-3</v>
-      </c>
-      <c r="F7" s="1">
-        <f t="shared" si="1"/>
-        <v>0.01</v>
-      </c>
-      <c r="G7" s="3"/>
-      <c r="I7" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A8">
-        <v>2</v>
-      </c>
-      <c r="B8" t="s">
-        <v>36</v>
-      </c>
-      <c r="C8" t="s">
-        <v>10</v>
-      </c>
-      <c r="D8">
-        <f t="shared" si="0"/>
-        <v>2000</v>
-      </c>
-      <c r="E8" s="1">
-        <v>5.0000000000000001E-3</v>
-      </c>
-      <c r="F8" s="1">
-        <f t="shared" si="1"/>
-        <v>0.01</v>
-      </c>
-      <c r="G8" s="3"/>
-      <c r="I8" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A9">
-        <v>2</v>
-      </c>
-      <c r="B9" t="s">
-        <v>37</v>
-      </c>
-      <c r="C9" t="s">
-        <v>38</v>
-      </c>
-      <c r="D9">
-        <f t="shared" ref="D9" si="2">1000*A9</f>
-        <v>2000</v>
-      </c>
-      <c r="E9" s="1">
-        <v>5.0000000000000001E-3</v>
-      </c>
-      <c r="F9" s="1">
-        <f t="shared" ref="F9" si="3">E9*A9</f>
-        <v>0.01</v>
-      </c>
-      <c r="G9" s="3"/>
-      <c r="I9" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="E10" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="F10" s="1"/>
-      <c r="G10" s="3"/>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A11">
-        <v>1</v>
-      </c>
-      <c r="B11" t="s">
-        <v>16</v>
-      </c>
-      <c r="D11">
-        <f t="shared" si="0"/>
-        <v>1000</v>
-      </c>
-      <c r="E11" s="1">
-        <v>300</v>
-      </c>
-      <c r="F11" s="1">
-        <f>E11/D11</f>
-        <v>0.3</v>
-      </c>
-      <c r="G11" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A12">
-        <v>1</v>
-      </c>
-      <c r="B12" t="s">
-        <v>17</v>
-      </c>
-      <c r="D12">
-        <f t="shared" si="0"/>
-        <v>1000</v>
-      </c>
-      <c r="E12" s="1">
-        <v>260</v>
-      </c>
-      <c r="F12" s="1">
-        <f t="shared" ref="F12:F13" si="4">E12/D12</f>
-        <v>0.26</v>
-      </c>
-      <c r="G12" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A13">
-        <v>1</v>
-      </c>
-      <c r="B13" t="s">
-        <v>31</v>
-      </c>
-      <c r="D13">
-        <v>1000</v>
-      </c>
-      <c r="E13" s="1">
-        <v>140</v>
-      </c>
-      <c r="F13" s="1">
-        <f t="shared" si="4"/>
-        <v>0.14000000000000001</v>
-      </c>
-      <c r="G13" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="G14" s="3"/>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="E15" t="s">
-        <v>20</v>
-      </c>
-      <c r="F15" s="1">
-        <f>SUM(F2:F13)</f>
-        <v>5.3599999999999985</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="E16" t="s">
-        <v>21</v>
-      </c>
-      <c r="F16" s="2">
-        <f>F15*1.1</f>
-        <v>5.895999999999999</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>